<commit_message>
Adding Unit 1 homework draft
</commit_message>
<xml_diff>
--- a/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/02-Ins_PivotTables/Solved/PivotTables.xlsx
+++ b/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/02-Ins_PivotTables/Solved/PivotTables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\2\Activities\09-Ins_PivotTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\Documents\GitHub\GWU-ARL-DATA-PT-09-2019-U-C\01-Class-Activities\Mon-Wed-Class\01-Excel\3\Activities\02-Ins_PivotTables\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="EB38C96A757F5A8F8FDBBC133FE1386DB659D6FE" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{B87C83CC-A6C0-4333-8D1D-521D4EE6FF64}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="20183" windowHeight="12818" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20190" windowHeight="12825" tabRatio="796"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,13 +19,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$214</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="31">
   <si>
     <t>Country</t>
   </si>
@@ -124,15 +123,21 @@
   <si>
     <t>Vegetables Total</t>
   </si>
+  <si>
+    <t>Can someone remind me how to do number formatting again?</t>
+  </si>
+  <si>
+    <t>I nominate Keishacarr! (You have to say her first and last name together) :-)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +147,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -182,11 +195,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -211,9 +250,9 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{FE0D9BC4-DAB8-496C-B826-44D3B596CAFA}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -228,7 +267,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jacob's Gaming Rig" refreshedDate="42873.827209490744" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="213" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jacob's Gaming Rig" refreshedDate="42873.827209490744" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="213">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F214" sheet="Sheet1"/>
   </cacheSource>
@@ -2140,7 +2179,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -2392,7 +2431,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -2491,6 +2530,21 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F214" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F214"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Order ID"/>
+    <tableColumn id="2" name="Product"/>
+    <tableColumn id="3" name="Category"/>
+    <tableColumn id="4" name="Profit" dataDxfId="2"/>
+    <tableColumn id="5" name="Date" dataDxfId="1"/>
+    <tableColumn id="6" name="Country"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2789,26 +2843,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.46484375" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2842,13 +2894,13 @@
         <v>4270</v>
       </c>
       <c r="E2" s="3">
-        <v>42375</v>
+        <v>43355</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2862,13 +2914,13 @@
         <v>8239</v>
       </c>
       <c r="E3" s="3">
-        <v>42376</v>
+        <v>43356</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2882,13 +2934,13 @@
         <v>617</v>
       </c>
       <c r="E4" s="3">
-        <v>42377</v>
+        <v>43357</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2902,13 +2954,13 @@
         <v>8384</v>
       </c>
       <c r="E5" s="3">
-        <v>42379</v>
+        <v>43359</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2922,13 +2974,13 @@
         <v>2626</v>
       </c>
       <c r="E6" s="3">
-        <v>42379</v>
+        <v>43359</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2942,13 +2994,13 @@
         <v>3610</v>
       </c>
       <c r="E7" s="3">
-        <v>42380</v>
+        <v>43360</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2962,13 +3014,13 @@
         <v>9062</v>
       </c>
       <c r="E8" s="3">
-        <v>42380</v>
+        <v>43360</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2982,13 +3034,13 @@
         <v>6906</v>
       </c>
       <c r="E9" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3002,13 +3054,13 @@
         <v>2417</v>
       </c>
       <c r="E10" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3022,13 +3074,13 @@
         <v>7431</v>
       </c>
       <c r="E11" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3042,13 +3094,13 @@
         <v>8250</v>
       </c>
       <c r="E12" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3062,13 +3114,13 @@
         <v>7012</v>
       </c>
       <c r="E13" s="3">
-        <v>42387</v>
+        <v>43367</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3082,13 +3134,13 @@
         <v>1903</v>
       </c>
       <c r="E14" s="3">
-        <v>42389</v>
+        <v>43369</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3102,13 +3154,13 @@
         <v>2824</v>
       </c>
       <c r="E15" s="3">
-        <v>42391</v>
+        <v>43371</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3122,13 +3174,13 @@
         <v>6946</v>
       </c>
       <c r="E16" s="3">
-        <v>42393</v>
+        <v>43373</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3142,13 +3194,13 @@
         <v>2320</v>
       </c>
       <c r="E17" s="3">
-        <v>42396</v>
+        <v>43376</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3162,13 +3214,13 @@
         <v>2116</v>
       </c>
       <c r="E18" s="3">
-        <v>42397</v>
+        <v>43377</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3182,13 +3234,13 @@
         <v>1135</v>
       </c>
       <c r="E19" s="3">
-        <v>42399</v>
+        <v>43379</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3202,13 +3254,13 @@
         <v>3595</v>
       </c>
       <c r="E20" s="3">
-        <v>42399</v>
+        <v>43379</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3222,13 +3274,13 @@
         <v>1161</v>
       </c>
       <c r="E21" s="3">
-        <v>42402</v>
+        <v>43382</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3242,13 +3294,13 @@
         <v>2256</v>
       </c>
       <c r="E22" s="3">
-        <v>42404</v>
+        <v>43384</v>
       </c>
       <c r="F22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3262,13 +3314,13 @@
         <v>1004</v>
       </c>
       <c r="E23" s="3">
-        <v>42411</v>
+        <v>43391</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3282,13 +3334,13 @@
         <v>3642</v>
       </c>
       <c r="E24" s="3">
-        <v>42414</v>
+        <v>43394</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3302,13 +3354,13 @@
         <v>4582</v>
       </c>
       <c r="E25" s="3">
-        <v>42417</v>
+        <v>43397</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3322,13 +3374,13 @@
         <v>3559</v>
       </c>
       <c r="E26" s="3">
-        <v>42417</v>
+        <v>43397</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3342,13 +3394,13 @@
         <v>5154</v>
       </c>
       <c r="E27" s="3">
-        <v>42417</v>
+        <v>43397</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3362,13 +3414,13 @@
         <v>7388</v>
       </c>
       <c r="E28" s="3">
-        <v>42418</v>
+        <v>43398</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3382,13 +3434,13 @@
         <v>7163</v>
       </c>
       <c r="E29" s="3">
-        <v>42418</v>
+        <v>43398</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3402,13 +3454,13 @@
         <v>5101</v>
       </c>
       <c r="E30" s="3">
-        <v>42420</v>
+        <v>43400</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3422,13 +3474,13 @@
         <v>7602</v>
       </c>
       <c r="E31" s="3">
-        <v>42421</v>
+        <v>43401</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3442,13 +3494,13 @@
         <v>1641</v>
       </c>
       <c r="E32" s="3">
-        <v>42422</v>
+        <v>43402</v>
       </c>
       <c r="F32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3462,13 +3514,13 @@
         <v>8892</v>
       </c>
       <c r="E33" s="3">
-        <v>42423</v>
+        <v>43403</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3482,13 +3534,13 @@
         <v>2060</v>
       </c>
       <c r="E34" s="3">
-        <v>42429</v>
+        <v>43409</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3502,13 +3554,13 @@
         <v>1557</v>
       </c>
       <c r="E35" s="3">
-        <v>42429</v>
+        <v>43409</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3522,13 +3574,13 @@
         <v>6509</v>
       </c>
       <c r="E36" s="3">
-        <v>42430</v>
+        <v>43410</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3542,13 +3594,13 @@
         <v>5718</v>
       </c>
       <c r="E37" s="3">
-        <v>42433</v>
+        <v>43413</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3562,13 +3614,13 @@
         <v>7655</v>
       </c>
       <c r="E38" s="3">
-        <v>42434</v>
+        <v>43414</v>
       </c>
       <c r="F38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3582,13 +3634,13 @@
         <v>9116</v>
       </c>
       <c r="E39" s="3">
-        <v>42434</v>
+        <v>43414</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3602,13 +3654,13 @@
         <v>2795</v>
       </c>
       <c r="E40" s="3">
-        <v>42444</v>
+        <v>43424</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3622,13 +3674,13 @@
         <v>5084</v>
       </c>
       <c r="E41" s="3">
-        <v>42444</v>
+        <v>43424</v>
       </c>
       <c r="F41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3642,13 +3694,13 @@
         <v>8941</v>
       </c>
       <c r="E42" s="3">
-        <v>42444</v>
+        <v>43424</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3662,13 +3714,13 @@
         <v>5341</v>
       </c>
       <c r="E43" s="3">
-        <v>42445</v>
+        <v>43425</v>
       </c>
       <c r="F43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3682,13 +3734,13 @@
         <v>135</v>
       </c>
       <c r="E44" s="3">
-        <v>42448</v>
+        <v>43428</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3702,13 +3754,13 @@
         <v>9400</v>
       </c>
       <c r="E45" s="3">
-        <v>42448</v>
+        <v>43428</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3722,13 +3774,13 @@
         <v>6045</v>
       </c>
       <c r="E46" s="3">
-        <v>42450</v>
+        <v>43430</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3742,13 +3794,13 @@
         <v>5820</v>
       </c>
       <c r="E47" s="3">
-        <v>42451</v>
+        <v>43431</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3762,13 +3814,13 @@
         <v>8887</v>
       </c>
       <c r="E48" s="3">
-        <v>42452</v>
+        <v>43432</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3782,13 +3834,13 @@
         <v>6982</v>
       </c>
       <c r="E49" s="3">
-        <v>42453</v>
+        <v>43433</v>
       </c>
       <c r="F49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3802,13 +3854,13 @@
         <v>4029</v>
       </c>
       <c r="E50" s="3">
-        <v>42455</v>
+        <v>43435</v>
       </c>
       <c r="F50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3822,13 +3874,13 @@
         <v>3665</v>
       </c>
       <c r="E51" s="3">
-        <v>42455</v>
+        <v>43435</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3842,13 +3894,13 @@
         <v>4781</v>
       </c>
       <c r="E52" s="3">
-        <v>42458</v>
+        <v>43438</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3862,13 +3914,13 @@
         <v>3663</v>
       </c>
       <c r="E53" s="3">
-        <v>42459</v>
+        <v>43439</v>
       </c>
       <c r="F53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3882,13 +3934,13 @@
         <v>6331</v>
       </c>
       <c r="E54" s="3">
-        <v>42461</v>
+        <v>43441</v>
       </c>
       <c r="F54" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3902,13 +3954,13 @@
         <v>4364</v>
       </c>
       <c r="E55" s="3">
-        <v>42461</v>
+        <v>43441</v>
       </c>
       <c r="F55" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3922,13 +3974,13 @@
         <v>607</v>
       </c>
       <c r="E56" s="3">
-        <v>42463</v>
+        <v>43443</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3942,13 +3994,13 @@
         <v>1054</v>
       </c>
       <c r="E57" s="3">
-        <v>42466</v>
+        <v>43446</v>
       </c>
       <c r="F57" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3962,13 +4014,13 @@
         <v>7659</v>
       </c>
       <c r="E58" s="3">
-        <v>42466</v>
+        <v>43446</v>
       </c>
       <c r="F58" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3982,13 +4034,13 @@
         <v>277</v>
       </c>
       <c r="E59" s="3">
-        <v>42472</v>
+        <v>43452</v>
       </c>
       <c r="F59" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4002,13 +4054,13 @@
         <v>235</v>
       </c>
       <c r="E60" s="3">
-        <v>42477</v>
+        <v>43457</v>
       </c>
       <c r="F60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4022,13 +4074,13 @@
         <v>1113</v>
       </c>
       <c r="E61" s="3">
-        <v>42478</v>
+        <v>43458</v>
       </c>
       <c r="F61" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4042,13 +4094,13 @@
         <v>1128</v>
       </c>
       <c r="E62" s="3">
-        <v>42481</v>
+        <v>43461</v>
       </c>
       <c r="F62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4062,13 +4114,13 @@
         <v>9231</v>
       </c>
       <c r="E63" s="3">
-        <v>42482</v>
+        <v>43462</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4082,13 +4134,13 @@
         <v>4387</v>
       </c>
       <c r="E64" s="3">
-        <v>42483</v>
+        <v>43463</v>
       </c>
       <c r="F64" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4102,13 +4154,13 @@
         <v>2763</v>
       </c>
       <c r="E65" s="3">
-        <v>42485</v>
+        <v>43465</v>
       </c>
       <c r="F65" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4122,13 +4174,13 @@
         <v>7898</v>
       </c>
       <c r="E66" s="3">
-        <v>42487</v>
+        <v>43467</v>
       </c>
       <c r="F66" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4142,13 +4194,13 @@
         <v>2427</v>
       </c>
       <c r="E67" s="3">
-        <v>42490</v>
+        <v>43470</v>
       </c>
       <c r="F67" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4162,13 +4214,13 @@
         <v>8663</v>
       </c>
       <c r="E68" s="3">
-        <v>42491</v>
+        <v>43471</v>
       </c>
       <c r="F68" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4182,13 +4234,13 @@
         <v>2789</v>
       </c>
       <c r="E69" s="3">
-        <v>42491</v>
+        <v>43471</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4202,13 +4254,13 @@
         <v>4054</v>
       </c>
       <c r="E70" s="3">
-        <v>42492</v>
+        <v>43472</v>
       </c>
       <c r="F70" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4222,13 +4274,13 @@
         <v>2262</v>
       </c>
       <c r="E71" s="3">
-        <v>42492</v>
+        <v>43472</v>
       </c>
       <c r="F71" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4242,13 +4294,13 @@
         <v>5600</v>
       </c>
       <c r="E72" s="3">
-        <v>42492</v>
+        <v>43472</v>
       </c>
       <c r="F72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4262,13 +4314,13 @@
         <v>5787</v>
       </c>
       <c r="E73" s="3">
-        <v>42493</v>
+        <v>43473</v>
       </c>
       <c r="F73" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4282,13 +4334,13 @@
         <v>6295</v>
       </c>
       <c r="E74" s="3">
-        <v>42493</v>
+        <v>43473</v>
       </c>
       <c r="F74" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4302,13 +4354,13 @@
         <v>474</v>
       </c>
       <c r="E75" s="3">
-        <v>42495</v>
+        <v>43475</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4322,13 +4374,13 @@
         <v>4325</v>
       </c>
       <c r="E76" s="3">
-        <v>42495</v>
+        <v>43475</v>
       </c>
       <c r="F76" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4342,13 +4394,13 @@
         <v>592</v>
       </c>
       <c r="E77" s="3">
-        <v>42496</v>
+        <v>43476</v>
       </c>
       <c r="F77" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4362,13 +4414,13 @@
         <v>4330</v>
       </c>
       <c r="E78" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F78" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4382,13 +4434,13 @@
         <v>9405</v>
       </c>
       <c r="E79" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F79" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4402,13 +4454,13 @@
         <v>7671</v>
       </c>
       <c r="E80" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4422,13 +4474,13 @@
         <v>5791</v>
       </c>
       <c r="E81" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F81" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4442,13 +4494,13 @@
         <v>6007</v>
       </c>
       <c r="E82" s="3">
-        <v>42502</v>
+        <v>43482</v>
       </c>
       <c r="F82" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4462,13 +4514,13 @@
         <v>5030</v>
       </c>
       <c r="E83" s="3">
-        <v>42504</v>
+        <v>43484</v>
       </c>
       <c r="F83" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4482,13 +4534,13 @@
         <v>6763</v>
       </c>
       <c r="E84" s="3">
-        <v>42504</v>
+        <v>43484</v>
       </c>
       <c r="F84" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4502,13 +4554,13 @@
         <v>4248</v>
       </c>
       <c r="E85" s="3">
-        <v>42505</v>
+        <v>43485</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4522,13 +4574,13 @@
         <v>9543</v>
       </c>
       <c r="E86" s="3">
-        <v>42506</v>
+        <v>43486</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4542,13 +4594,13 @@
         <v>2054</v>
       </c>
       <c r="E87" s="3">
-        <v>42506</v>
+        <v>43486</v>
       </c>
       <c r="F87" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4562,13 +4614,13 @@
         <v>7094</v>
       </c>
       <c r="E88" s="3">
-        <v>42506</v>
+        <v>43486</v>
       </c>
       <c r="F88" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4582,13 +4634,13 @@
         <v>6087</v>
       </c>
       <c r="E89" s="3">
-        <v>42508</v>
+        <v>43488</v>
       </c>
       <c r="F89" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4602,13 +4654,13 @@
         <v>4264</v>
       </c>
       <c r="E90" s="3">
-        <v>42509</v>
+        <v>43489</v>
       </c>
       <c r="F90" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4622,13 +4674,13 @@
         <v>9333</v>
       </c>
       <c r="E91" s="3">
-        <v>42510</v>
+        <v>43490</v>
       </c>
       <c r="F91" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4642,13 +4694,13 @@
         <v>8775</v>
       </c>
       <c r="E92" s="3">
-        <v>42512</v>
+        <v>43492</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4662,13 +4714,13 @@
         <v>2011</v>
       </c>
       <c r="E93" s="3">
-        <v>42513</v>
+        <v>43493</v>
       </c>
       <c r="F93" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4682,13 +4734,13 @@
         <v>5632</v>
       </c>
       <c r="E94" s="3">
-        <v>42515</v>
+        <v>43495</v>
       </c>
       <c r="F94" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4702,13 +4754,13 @@
         <v>4904</v>
       </c>
       <c r="E95" s="3">
-        <v>42515</v>
+        <v>43495</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4722,13 +4774,13 @@
         <v>1002</v>
       </c>
       <c r="E96" s="3">
-        <v>42515</v>
+        <v>43495</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4742,13 +4794,13 @@
         <v>8141</v>
       </c>
       <c r="E97" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F97" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4762,13 +4814,13 @@
         <v>3644</v>
       </c>
       <c r="E98" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F98" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4782,13 +4834,13 @@
         <v>1380</v>
       </c>
       <c r="E99" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4802,13 +4854,13 @@
         <v>8354</v>
       </c>
       <c r="E100" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4822,13 +4874,13 @@
         <v>5182</v>
       </c>
       <c r="E101" s="3">
-        <v>42517</v>
+        <v>43497</v>
       </c>
       <c r="F101" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4842,13 +4894,13 @@
         <v>2193</v>
       </c>
       <c r="E102" s="3">
-        <v>42517</v>
+        <v>43497</v>
       </c>
       <c r="F102" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4862,13 +4914,13 @@
         <v>3647</v>
       </c>
       <c r="E103" s="3">
-        <v>42518</v>
+        <v>43498</v>
       </c>
       <c r="F103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4882,13 +4934,13 @@
         <v>4104</v>
       </c>
       <c r="E104" s="3">
-        <v>42518</v>
+        <v>43498</v>
       </c>
       <c r="F104" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4902,13 +4954,13 @@
         <v>7457</v>
       </c>
       <c r="E105" s="3">
-        <v>42518</v>
+        <v>43498</v>
       </c>
       <c r="F105" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4922,13 +4974,13 @@
         <v>3767</v>
       </c>
       <c r="E106" s="3">
-        <v>42519</v>
+        <v>43499</v>
       </c>
       <c r="F106" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4942,13 +4994,13 @@
         <v>4685</v>
       </c>
       <c r="E107" s="3">
-        <v>42520</v>
+        <v>43500</v>
       </c>
       <c r="F107" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4962,13 +5014,13 @@
         <v>3917</v>
       </c>
       <c r="E108" s="3">
-        <v>42525</v>
+        <v>43505</v>
       </c>
       <c r="F108" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4982,13 +5034,13 @@
         <v>521</v>
       </c>
       <c r="E109" s="3">
-        <v>42525</v>
+        <v>43505</v>
       </c>
       <c r="F109" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5002,13 +5054,13 @@
         <v>5605</v>
       </c>
       <c r="E110" s="3">
-        <v>42531</v>
+        <v>43511</v>
       </c>
       <c r="F110" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5022,13 +5074,13 @@
         <v>9630</v>
       </c>
       <c r="E111" s="3">
-        <v>42532</v>
+        <v>43512</v>
       </c>
       <c r="F111" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5042,13 +5094,13 @@
         <v>6941</v>
       </c>
       <c r="E112" s="3">
-        <v>42541</v>
+        <v>43521</v>
       </c>
       <c r="F112" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5062,13 +5114,13 @@
         <v>7231</v>
       </c>
       <c r="E113" s="3">
-        <v>42541</v>
+        <v>43521</v>
       </c>
       <c r="F113" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5082,13 +5134,13 @@
         <v>8891</v>
       </c>
       <c r="E114" s="3">
-        <v>42544</v>
+        <v>43524</v>
       </c>
       <c r="F114" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5102,13 +5154,13 @@
         <v>107</v>
       </c>
       <c r="E115" s="3">
-        <v>42546</v>
+        <v>43526</v>
       </c>
       <c r="F115" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5122,13 +5174,13 @@
         <v>4243</v>
       </c>
       <c r="E116" s="3">
-        <v>42547</v>
+        <v>43527</v>
       </c>
       <c r="F116" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5142,13 +5194,13 @@
         <v>4514</v>
       </c>
       <c r="E117" s="3">
-        <v>42548</v>
+        <v>43528</v>
       </c>
       <c r="F117" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5162,13 +5214,13 @@
         <v>5480</v>
       </c>
       <c r="E118" s="3">
-        <v>42553</v>
+        <v>43533</v>
       </c>
       <c r="F118" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5182,13 +5234,13 @@
         <v>5002</v>
       </c>
       <c r="E119" s="3">
-        <v>42553</v>
+        <v>43533</v>
       </c>
       <c r="F119" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5202,13 +5254,13 @@
         <v>8530</v>
       </c>
       <c r="E120" s="3">
-        <v>42556</v>
+        <v>43536</v>
       </c>
       <c r="F120" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5222,13 +5274,13 @@
         <v>4819</v>
       </c>
       <c r="E121" s="3">
-        <v>42558</v>
+        <v>43538</v>
       </c>
       <c r="F121" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5242,13 +5294,13 @@
         <v>6343</v>
       </c>
       <c r="E122" s="3">
-        <v>42562</v>
+        <v>43542</v>
       </c>
       <c r="F122" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5262,13 +5314,13 @@
         <v>2318</v>
       </c>
       <c r="E123" s="3">
-        <v>42564</v>
+        <v>43544</v>
       </c>
       <c r="F123" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5282,13 +5334,13 @@
         <v>220</v>
       </c>
       <c r="E124" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F124" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5302,13 +5354,13 @@
         <v>6341</v>
       </c>
       <c r="E125" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F125" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5322,13 +5374,13 @@
         <v>330</v>
       </c>
       <c r="E126" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F126" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5342,13 +5394,13 @@
         <v>3027</v>
       </c>
       <c r="E127" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F127" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5362,13 +5414,13 @@
         <v>850</v>
       </c>
       <c r="E128" s="3">
-        <v>42573</v>
+        <v>43553</v>
       </c>
       <c r="F128" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5382,13 +5434,13 @@
         <v>8986</v>
       </c>
       <c r="E129" s="3">
-        <v>42574</v>
+        <v>43554</v>
       </c>
       <c r="F129" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5402,13 +5454,13 @@
         <v>3800</v>
       </c>
       <c r="E130" s="3">
-        <v>42576</v>
+        <v>43556</v>
       </c>
       <c r="F130" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5422,13 +5474,13 @@
         <v>5751</v>
       </c>
       <c r="E131" s="3">
-        <v>42579</v>
+        <v>43559</v>
       </c>
       <c r="F131" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5442,13 +5494,13 @@
         <v>1704</v>
       </c>
       <c r="E132" s="3">
-        <v>42580</v>
+        <v>43560</v>
       </c>
       <c r="F132" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5462,13 +5514,13 @@
         <v>7966</v>
       </c>
       <c r="E133" s="3">
-        <v>42581</v>
+        <v>43561</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5482,13 +5534,13 @@
         <v>852</v>
       </c>
       <c r="E134" s="3">
-        <v>42582</v>
+        <v>43562</v>
       </c>
       <c r="F134" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5502,13 +5554,13 @@
         <v>8416</v>
       </c>
       <c r="E135" s="3">
-        <v>42582</v>
+        <v>43562</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5522,13 +5574,13 @@
         <v>7144</v>
       </c>
       <c r="E136" s="3">
-        <v>42583</v>
+        <v>43563</v>
       </c>
       <c r="F136" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5542,13 +5594,13 @@
         <v>7854</v>
       </c>
       <c r="E137" s="3">
-        <v>42583</v>
+        <v>43563</v>
       </c>
       <c r="F137" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5562,13 +5614,13 @@
         <v>859</v>
       </c>
       <c r="E138" s="3">
-        <v>42585</v>
+        <v>43565</v>
       </c>
       <c r="F138" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5582,13 +5634,13 @@
         <v>8049</v>
       </c>
       <c r="E139" s="3">
-        <v>42594</v>
+        <v>43574</v>
       </c>
       <c r="F139" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5602,13 +5654,13 @@
         <v>2836</v>
       </c>
       <c r="E140" s="3">
-        <v>42595</v>
+        <v>43575</v>
       </c>
       <c r="F140" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5622,13 +5674,13 @@
         <v>1743</v>
       </c>
       <c r="E141" s="3">
-        <v>42601</v>
+        <v>43581</v>
       </c>
       <c r="F141" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5642,13 +5694,13 @@
         <v>3844</v>
       </c>
       <c r="E142" s="3">
-        <v>42605</v>
+        <v>43585</v>
       </c>
       <c r="F142" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5662,13 +5714,13 @@
         <v>7490</v>
       </c>
       <c r="E143" s="3">
-        <v>42606</v>
+        <v>43586</v>
       </c>
       <c r="F143" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5682,13 +5734,13 @@
         <v>4483</v>
       </c>
       <c r="E144" s="3">
-        <v>42607</v>
+        <v>43587</v>
       </c>
       <c r="F144" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5702,13 +5754,13 @@
         <v>7333</v>
       </c>
       <c r="E145" s="3">
-        <v>42609</v>
+        <v>43589</v>
       </c>
       <c r="F145" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5722,13 +5774,13 @@
         <v>7654</v>
       </c>
       <c r="E146" s="3">
-        <v>42610</v>
+        <v>43590</v>
       </c>
       <c r="F146" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5742,13 +5794,13 @@
         <v>3944</v>
       </c>
       <c r="E147" s="3">
-        <v>42611</v>
+        <v>43591</v>
       </c>
       <c r="F147" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5762,13 +5814,13 @@
         <v>5761</v>
       </c>
       <c r="E148" s="3">
-        <v>42611</v>
+        <v>43591</v>
       </c>
       <c r="F148" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5782,13 +5834,13 @@
         <v>6864</v>
       </c>
       <c r="E149" s="3">
-        <v>42614</v>
+        <v>43594</v>
       </c>
       <c r="F149" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5802,13 +5854,13 @@
         <v>4016</v>
       </c>
       <c r="E150" s="3">
-        <v>42614</v>
+        <v>43594</v>
       </c>
       <c r="F150" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5822,13 +5874,13 @@
         <v>1841</v>
       </c>
       <c r="E151" s="3">
-        <v>42615</v>
+        <v>43595</v>
       </c>
       <c r="F151" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5842,13 +5894,13 @@
         <v>424</v>
       </c>
       <c r="E152" s="3">
-        <v>42618</v>
+        <v>43598</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5862,13 +5914,13 @@
         <v>8765</v>
       </c>
       <c r="E153" s="3">
-        <v>42620</v>
+        <v>43600</v>
       </c>
       <c r="F153" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5882,13 +5934,13 @@
         <v>5583</v>
       </c>
       <c r="E154" s="3">
-        <v>42621</v>
+        <v>43601</v>
       </c>
       <c r="F154" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5902,13 +5954,13 @@
         <v>4390</v>
       </c>
       <c r="E155" s="3">
-        <v>42622</v>
+        <v>43602</v>
       </c>
       <c r="F155" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5922,13 +5974,13 @@
         <v>352</v>
       </c>
       <c r="E156" s="3">
-        <v>42622</v>
+        <v>43602</v>
       </c>
       <c r="F156" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5942,13 +5994,13 @@
         <v>8489</v>
       </c>
       <c r="E157" s="3">
-        <v>42624</v>
+        <v>43604</v>
       </c>
       <c r="F157" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5962,13 +6014,13 @@
         <v>7090</v>
       </c>
       <c r="E158" s="3">
-        <v>42624</v>
+        <v>43604</v>
       </c>
       <c r="F158" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5982,13 +6034,13 @@
         <v>7880</v>
       </c>
       <c r="E159" s="3">
-        <v>42628</v>
+        <v>43608</v>
       </c>
       <c r="F159" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6002,13 +6054,13 @@
         <v>3861</v>
       </c>
       <c r="E160" s="3">
-        <v>42631</v>
+        <v>43611</v>
       </c>
       <c r="F160" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6022,13 +6074,13 @@
         <v>7927</v>
       </c>
       <c r="E161" s="3">
-        <v>42632</v>
+        <v>43612</v>
       </c>
       <c r="F161" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6042,13 +6094,13 @@
         <v>6162</v>
       </c>
       <c r="E162" s="3">
-        <v>42633</v>
+        <v>43613</v>
       </c>
       <c r="F162" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6062,13 +6114,13 @@
         <v>5523</v>
       </c>
       <c r="E163" s="3">
-        <v>42638</v>
+        <v>43618</v>
       </c>
       <c r="F163" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6082,13 +6134,13 @@
         <v>5936</v>
       </c>
       <c r="E164" s="3">
-        <v>42638</v>
+        <v>43618</v>
       </c>
       <c r="F164" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6102,13 +6154,13 @@
         <v>7251</v>
       </c>
       <c r="E165" s="3">
-        <v>42639</v>
+        <v>43619</v>
       </c>
       <c r="F165" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6122,13 +6174,13 @@
         <v>6187</v>
       </c>
       <c r="E166" s="3">
-        <v>42640</v>
+        <v>43620</v>
       </c>
       <c r="F166" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6142,13 +6194,13 @@
         <v>3210</v>
       </c>
       <c r="E167" s="3">
-        <v>42642</v>
+        <v>43622</v>
       </c>
       <c r="F167" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6162,13 +6214,13 @@
         <v>682</v>
       </c>
       <c r="E168" s="3">
-        <v>42642</v>
+        <v>43622</v>
       </c>
       <c r="F168" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6182,13 +6234,13 @@
         <v>793</v>
       </c>
       <c r="E169" s="3">
-        <v>42646</v>
+        <v>43626</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6202,13 +6254,13 @@
         <v>5346</v>
       </c>
       <c r="E170" s="3">
-        <v>42647</v>
+        <v>43627</v>
       </c>
       <c r="F170" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6222,13 +6274,13 @@
         <v>7103</v>
       </c>
       <c r="E171" s="3">
-        <v>42650</v>
+        <v>43630</v>
       </c>
       <c r="F171" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6242,13 +6294,13 @@
         <v>4603</v>
       </c>
       <c r="E172" s="3">
-        <v>42653</v>
+        <v>43633</v>
       </c>
       <c r="F172" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6262,13 +6314,13 @@
         <v>8160</v>
       </c>
       <c r="E173" s="3">
-        <v>42659</v>
+        <v>43639</v>
       </c>
       <c r="F173" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6282,13 +6334,13 @@
         <v>7171</v>
       </c>
       <c r="E174" s="3">
-        <v>42666</v>
+        <v>43646</v>
       </c>
       <c r="F174" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6302,13 +6354,13 @@
         <v>3552</v>
       </c>
       <c r="E175" s="3">
-        <v>42666</v>
+        <v>43646</v>
       </c>
       <c r="F175" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6322,13 +6374,13 @@
         <v>7273</v>
       </c>
       <c r="E176" s="3">
-        <v>42668</v>
+        <v>43648</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6342,13 +6394,13 @@
         <v>2402</v>
       </c>
       <c r="E177" s="3">
-        <v>42669</v>
+        <v>43649</v>
       </c>
       <c r="F177" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6362,13 +6414,13 @@
         <v>1197</v>
       </c>
       <c r="E178" s="3">
-        <v>42669</v>
+        <v>43649</v>
       </c>
       <c r="F178" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6382,13 +6434,13 @@
         <v>5015</v>
       </c>
       <c r="E179" s="3">
-        <v>42669</v>
+        <v>43649</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6402,13 +6454,13 @@
         <v>5818</v>
       </c>
       <c r="E180" s="3">
-        <v>42676</v>
+        <v>43656</v>
       </c>
       <c r="F180" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6422,13 +6474,13 @@
         <v>4399</v>
       </c>
       <c r="E181" s="3">
-        <v>42677</v>
+        <v>43657</v>
       </c>
       <c r="F181" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6442,13 +6494,13 @@
         <v>3011</v>
       </c>
       <c r="E182" s="3">
-        <v>42677</v>
+        <v>43657</v>
       </c>
       <c r="F182" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -6462,13 +6514,13 @@
         <v>4715</v>
       </c>
       <c r="E183" s="3">
-        <v>42683</v>
+        <v>43663</v>
       </c>
       <c r="F183" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6482,13 +6534,13 @@
         <v>5321</v>
       </c>
       <c r="E184" s="3">
-        <v>42686</v>
+        <v>43666</v>
       </c>
       <c r="F184" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6502,13 +6554,13 @@
         <v>8894</v>
       </c>
       <c r="E185" s="3">
-        <v>42689</v>
+        <v>43669</v>
       </c>
       <c r="F185" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6522,13 +6574,13 @@
         <v>4846</v>
       </c>
       <c r="E186" s="3">
-        <v>42699</v>
+        <v>43679</v>
       </c>
       <c r="F186" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6542,13 +6594,13 @@
         <v>284</v>
       </c>
       <c r="E187" s="3">
-        <v>42699</v>
+        <v>43679</v>
       </c>
       <c r="F187" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -6562,13 +6614,13 @@
         <v>8283</v>
       </c>
       <c r="E188" s="3">
-        <v>42700</v>
+        <v>43680</v>
       </c>
       <c r="F188" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6582,13 +6634,13 @@
         <v>9990</v>
       </c>
       <c r="E189" s="3">
-        <v>42702</v>
+        <v>43682</v>
       </c>
       <c r="F189" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6602,13 +6654,13 @@
         <v>9014</v>
       </c>
       <c r="E190" s="3">
-        <v>42702</v>
+        <v>43682</v>
       </c>
       <c r="F190" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -6622,13 +6674,13 @@
         <v>1942</v>
       </c>
       <c r="E191" s="3">
-        <v>42703</v>
+        <v>43683</v>
       </c>
       <c r="F191" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6642,13 +6694,13 @@
         <v>7223</v>
       </c>
       <c r="E192" s="3">
-        <v>42704</v>
+        <v>43684</v>
       </c>
       <c r="F192" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6662,13 +6714,13 @@
         <v>4673</v>
       </c>
       <c r="E193" s="3">
-        <v>42706</v>
+        <v>43686</v>
       </c>
       <c r="F193" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6682,13 +6734,13 @@
         <v>9104</v>
       </c>
       <c r="E194" s="3">
-        <v>42708</v>
+        <v>43688</v>
       </c>
       <c r="F194" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6702,13 +6754,13 @@
         <v>6078</v>
       </c>
       <c r="E195" s="3">
-        <v>42709</v>
+        <v>43689</v>
       </c>
       <c r="F195" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6722,13 +6774,13 @@
         <v>3278</v>
       </c>
       <c r="E196" s="3">
-        <v>42710</v>
+        <v>43690</v>
       </c>
       <c r="F196" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6742,13 +6794,13 @@
         <v>136</v>
       </c>
       <c r="E197" s="3">
-        <v>42716</v>
+        <v>43696</v>
       </c>
       <c r="F197" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6762,13 +6814,13 @@
         <v>8377</v>
       </c>
       <c r="E198" s="3">
-        <v>42716</v>
+        <v>43696</v>
       </c>
       <c r="F198" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6782,13 +6834,13 @@
         <v>2382</v>
       </c>
       <c r="E199" s="3">
-        <v>42716</v>
+        <v>43696</v>
       </c>
       <c r="F199" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6802,13 +6854,13 @@
         <v>8702</v>
       </c>
       <c r="E200" s="3">
-        <v>42719</v>
+        <v>43699</v>
       </c>
       <c r="F200" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6822,13 +6874,13 @@
         <v>5021</v>
       </c>
       <c r="E201" s="3">
-        <v>42720</v>
+        <v>43700</v>
       </c>
       <c r="F201" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6842,13 +6894,13 @@
         <v>1760</v>
       </c>
       <c r="E202" s="3">
-        <v>42720</v>
+        <v>43700</v>
       </c>
       <c r="F202" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6862,13 +6914,13 @@
         <v>4766</v>
       </c>
       <c r="E203" s="3">
-        <v>42722</v>
+        <v>43702</v>
       </c>
       <c r="F203" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6882,13 +6934,13 @@
         <v>1541</v>
       </c>
       <c r="E204" s="3">
-        <v>42723</v>
+        <v>43703</v>
       </c>
       <c r="F204" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6902,13 +6954,13 @@
         <v>2782</v>
       </c>
       <c r="E205" s="3">
-        <v>42724</v>
+        <v>43704</v>
       </c>
       <c r="F205" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6922,13 +6974,13 @@
         <v>2455</v>
       </c>
       <c r="E206" s="3">
-        <v>42724</v>
+        <v>43704</v>
       </c>
       <c r="F206" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6942,13 +6994,13 @@
         <v>4512</v>
       </c>
       <c r="E207" s="3">
-        <v>42726</v>
+        <v>43706</v>
       </c>
       <c r="F207" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6962,13 +7014,13 @@
         <v>8752</v>
       </c>
       <c r="E208" s="3">
-        <v>42726</v>
+        <v>43706</v>
       </c>
       <c r="F208" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6982,13 +7034,13 @@
         <v>9127</v>
       </c>
       <c r="E209" s="3">
-        <v>42729</v>
+        <v>43709</v>
       </c>
       <c r="F209" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -7002,13 +7054,13 @@
         <v>1777</v>
       </c>
       <c r="E210" s="3">
-        <v>42732</v>
+        <v>43712</v>
       </c>
       <c r="F210" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -7022,13 +7074,13 @@
         <v>680</v>
       </c>
       <c r="E211" s="3">
-        <v>42732</v>
+        <v>43712</v>
       </c>
       <c r="F211" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -7042,13 +7094,13 @@
         <v>958</v>
       </c>
       <c r="E212" s="3">
-        <v>42733</v>
+        <v>43713</v>
       </c>
       <c r="F212" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -7062,13 +7114,13 @@
         <v>2613</v>
       </c>
       <c r="E213" s="3">
-        <v>42733</v>
+        <v>43713</v>
       </c>
       <c r="F213" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -7082,7 +7134,7 @@
         <v>339</v>
       </c>
       <c r="E214" s="3">
-        <v>42734</v>
+        <v>43714</v>
       </c>
       <c r="F214" t="s">
         <v>10</v>
@@ -7091,25 +7143,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -7117,7 +7170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -7128,7 +7181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -7139,7 +7192,7 @@
         <v>8892</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -7150,7 +7203,7 @@
         <v>9543</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -7161,7 +7214,7 @@
         <v>8416</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -7172,7 +7225,7 @@
         <v>9630</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -7183,7 +7236,7 @@
         <v>9127</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -7194,7 +7247,7 @@
         <v>9333</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -7205,7 +7258,7 @@
         <v>9990</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -7214,6 +7267,16 @@
       </c>
       <c r="C12" s="4">
         <v>9990</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -7222,20 +7285,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7243,7 +7304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -7251,13 +7312,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -7265,7 +7326,7 @@
         <v>191257</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -7273,7 +7334,7 @@
         <v>340295</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -7281,7 +7342,7 @@
         <v>57079</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -7289,7 +7350,7 @@
         <v>104438</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
@@ -7297,13 +7358,13 @@
         <v>693069</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
@@ -7311,7 +7372,7 @@
         <v>57281</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -7319,7 +7380,7 @@
         <v>142439</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -7327,7 +7388,7 @@
         <v>136945</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -7335,7 +7396,7 @@
         <v>336665</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Revert "Adding Unit 1 homework draft"
This reverts commit cc08d46ff4010f7f6a6de24270dbd7ec4a5197d2.
</commit_message>
<xml_diff>
--- a/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/02-Ins_PivotTables/Solved/PivotTables.xlsx
+++ b/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/02-Ins_PivotTables/Solved/PivotTables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\Documents\GitHub\GWU-ARL-DATA-PT-09-2019-U-C\01-Class-Activities\Mon-Wed-Class\01-Excel\3\Activities\02-Ins_PivotTables\Solved\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\2\Activities\09-Ins_PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="EB38C96A757F5A8F8FDBBC133FE1386DB659D6FE" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{B87C83CC-A6C0-4333-8D1D-521D4EE6FF64}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20190" windowHeight="12825" tabRatio="796"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="20183" windowHeight="12818" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,13 +20,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$214</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="29">
   <si>
     <t>Country</t>
   </si>
@@ -123,21 +124,15 @@
   <si>
     <t>Vegetables Total</t>
   </si>
-  <si>
-    <t>Can someone remind me how to do number formatting again?</t>
-  </si>
-  <si>
-    <t>I nominate Keishacarr! (You have to say her first and last name together) :-)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,14 +142,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -182,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -195,37 +182,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b/>
@@ -250,9 +211,9 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="3"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{FE0D9BC4-DAB8-496C-B826-44D3B596CAFA}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -267,7 +228,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jacob's Gaming Rig" refreshedDate="42873.827209490744" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="213">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jacob's Gaming Rig" refreshedDate="42873.827209490744" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="213" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F214" sheet="Sheet1"/>
   </cacheSource>
@@ -2179,7 +2140,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -2431,7 +2392,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -2530,21 +2491,6 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F214" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F214"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Order ID"/>
-    <tableColumn id="2" name="Product"/>
-    <tableColumn id="3" name="Category"/>
-    <tableColumn id="4" name="Profit" dataDxfId="2"/>
-    <tableColumn id="5" name="Date" dataDxfId="1"/>
-    <tableColumn id="6" name="Country"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2843,24 +2789,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="1" max="1" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.46484375" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2880,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2894,13 +2842,13 @@
         <v>4270</v>
       </c>
       <c r="E2" s="3">
-        <v>43355</v>
+        <v>42375</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2914,13 +2862,13 @@
         <v>8239</v>
       </c>
       <c r="E3" s="3">
-        <v>43356</v>
+        <v>42376</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2934,13 +2882,13 @@
         <v>617</v>
       </c>
       <c r="E4" s="3">
-        <v>43357</v>
+        <v>42377</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2954,13 +2902,13 @@
         <v>8384</v>
       </c>
       <c r="E5" s="3">
-        <v>43359</v>
+        <v>42379</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2974,13 +2922,13 @@
         <v>2626</v>
       </c>
       <c r="E6" s="3">
-        <v>43359</v>
+        <v>42379</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2994,13 +2942,13 @@
         <v>3610</v>
       </c>
       <c r="E7" s="3">
-        <v>43360</v>
+        <v>42380</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3014,13 +2962,13 @@
         <v>9062</v>
       </c>
       <c r="E8" s="3">
-        <v>43360</v>
+        <v>42380</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3034,13 +2982,13 @@
         <v>6906</v>
       </c>
       <c r="E9" s="3">
-        <v>43365</v>
+        <v>42385</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3054,13 +3002,13 @@
         <v>2417</v>
       </c>
       <c r="E10" s="3">
-        <v>43365</v>
+        <v>42385</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3074,13 +3022,13 @@
         <v>7431</v>
       </c>
       <c r="E11" s="3">
-        <v>43365</v>
+        <v>42385</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3094,13 +3042,13 @@
         <v>8250</v>
       </c>
       <c r="E12" s="3">
-        <v>43365</v>
+        <v>42385</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3114,13 +3062,13 @@
         <v>7012</v>
       </c>
       <c r="E13" s="3">
-        <v>43367</v>
+        <v>42387</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3134,13 +3082,13 @@
         <v>1903</v>
       </c>
       <c r="E14" s="3">
-        <v>43369</v>
+        <v>42389</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3154,13 +3102,13 @@
         <v>2824</v>
       </c>
       <c r="E15" s="3">
-        <v>43371</v>
+        <v>42391</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3174,13 +3122,13 @@
         <v>6946</v>
       </c>
       <c r="E16" s="3">
-        <v>43373</v>
+        <v>42393</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3194,13 +3142,13 @@
         <v>2320</v>
       </c>
       <c r="E17" s="3">
-        <v>43376</v>
+        <v>42396</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3214,13 +3162,13 @@
         <v>2116</v>
       </c>
       <c r="E18" s="3">
-        <v>43377</v>
+        <v>42397</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3234,13 +3182,13 @@
         <v>1135</v>
       </c>
       <c r="E19" s="3">
-        <v>43379</v>
+        <v>42399</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3254,13 +3202,13 @@
         <v>3595</v>
       </c>
       <c r="E20" s="3">
-        <v>43379</v>
+        <v>42399</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3274,13 +3222,13 @@
         <v>1161</v>
       </c>
       <c r="E21" s="3">
-        <v>43382</v>
+        <v>42402</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3294,13 +3242,13 @@
         <v>2256</v>
       </c>
       <c r="E22" s="3">
-        <v>43384</v>
+        <v>42404</v>
       </c>
       <c r="F22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3314,13 +3262,13 @@
         <v>1004</v>
       </c>
       <c r="E23" s="3">
-        <v>43391</v>
+        <v>42411</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3334,13 +3282,13 @@
         <v>3642</v>
       </c>
       <c r="E24" s="3">
-        <v>43394</v>
+        <v>42414</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3354,13 +3302,13 @@
         <v>4582</v>
       </c>
       <c r="E25" s="3">
-        <v>43397</v>
+        <v>42417</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3374,13 +3322,13 @@
         <v>3559</v>
       </c>
       <c r="E26" s="3">
-        <v>43397</v>
+        <v>42417</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3394,13 +3342,13 @@
         <v>5154</v>
       </c>
       <c r="E27" s="3">
-        <v>43397</v>
+        <v>42417</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3414,13 +3362,13 @@
         <v>7388</v>
       </c>
       <c r="E28" s="3">
-        <v>43398</v>
+        <v>42418</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3434,13 +3382,13 @@
         <v>7163</v>
       </c>
       <c r="E29" s="3">
-        <v>43398</v>
+        <v>42418</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3454,13 +3402,13 @@
         <v>5101</v>
       </c>
       <c r="E30" s="3">
-        <v>43400</v>
+        <v>42420</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3474,13 +3422,13 @@
         <v>7602</v>
       </c>
       <c r="E31" s="3">
-        <v>43401</v>
+        <v>42421</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3494,13 +3442,13 @@
         <v>1641</v>
       </c>
       <c r="E32" s="3">
-        <v>43402</v>
+        <v>42422</v>
       </c>
       <c r="F32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3514,13 +3462,13 @@
         <v>8892</v>
       </c>
       <c r="E33" s="3">
-        <v>43403</v>
+        <v>42423</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3534,13 +3482,13 @@
         <v>2060</v>
       </c>
       <c r="E34" s="3">
-        <v>43409</v>
+        <v>42429</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3554,13 +3502,13 @@
         <v>1557</v>
       </c>
       <c r="E35" s="3">
-        <v>43409</v>
+        <v>42429</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3574,13 +3522,13 @@
         <v>6509</v>
       </c>
       <c r="E36" s="3">
-        <v>43410</v>
+        <v>42430</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3594,13 +3542,13 @@
         <v>5718</v>
       </c>
       <c r="E37" s="3">
-        <v>43413</v>
+        <v>42433</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3614,13 +3562,13 @@
         <v>7655</v>
       </c>
       <c r="E38" s="3">
-        <v>43414</v>
+        <v>42434</v>
       </c>
       <c r="F38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3634,13 +3582,13 @@
         <v>9116</v>
       </c>
       <c r="E39" s="3">
-        <v>43414</v>
+        <v>42434</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3654,13 +3602,13 @@
         <v>2795</v>
       </c>
       <c r="E40" s="3">
-        <v>43424</v>
+        <v>42444</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3674,13 +3622,13 @@
         <v>5084</v>
       </c>
       <c r="E41" s="3">
-        <v>43424</v>
+        <v>42444</v>
       </c>
       <c r="F41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3694,13 +3642,13 @@
         <v>8941</v>
       </c>
       <c r="E42" s="3">
-        <v>43424</v>
+        <v>42444</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3714,13 +3662,13 @@
         <v>5341</v>
       </c>
       <c r="E43" s="3">
-        <v>43425</v>
+        <v>42445</v>
       </c>
       <c r="F43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3734,13 +3682,13 @@
         <v>135</v>
       </c>
       <c r="E44" s="3">
-        <v>43428</v>
+        <v>42448</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3754,13 +3702,13 @@
         <v>9400</v>
       </c>
       <c r="E45" s="3">
-        <v>43428</v>
+        <v>42448</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3774,13 +3722,13 @@
         <v>6045</v>
       </c>
       <c r="E46" s="3">
-        <v>43430</v>
+        <v>42450</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3794,13 +3742,13 @@
         <v>5820</v>
       </c>
       <c r="E47" s="3">
-        <v>43431</v>
+        <v>42451</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3814,13 +3762,13 @@
         <v>8887</v>
       </c>
       <c r="E48" s="3">
-        <v>43432</v>
+        <v>42452</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3834,13 +3782,13 @@
         <v>6982</v>
       </c>
       <c r="E49" s="3">
-        <v>43433</v>
+        <v>42453</v>
       </c>
       <c r="F49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3854,13 +3802,13 @@
         <v>4029</v>
       </c>
       <c r="E50" s="3">
-        <v>43435</v>
+        <v>42455</v>
       </c>
       <c r="F50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3874,13 +3822,13 @@
         <v>3665</v>
       </c>
       <c r="E51" s="3">
-        <v>43435</v>
+        <v>42455</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3894,13 +3842,13 @@
         <v>4781</v>
       </c>
       <c r="E52" s="3">
-        <v>43438</v>
+        <v>42458</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3914,13 +3862,13 @@
         <v>3663</v>
       </c>
       <c r="E53" s="3">
-        <v>43439</v>
+        <v>42459</v>
       </c>
       <c r="F53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3934,13 +3882,13 @@
         <v>6331</v>
       </c>
       <c r="E54" s="3">
-        <v>43441</v>
+        <v>42461</v>
       </c>
       <c r="F54" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3954,13 +3902,13 @@
         <v>4364</v>
       </c>
       <c r="E55" s="3">
-        <v>43441</v>
+        <v>42461</v>
       </c>
       <c r="F55" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3974,13 +3922,13 @@
         <v>607</v>
       </c>
       <c r="E56" s="3">
-        <v>43443</v>
+        <v>42463</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3994,13 +3942,13 @@
         <v>1054</v>
       </c>
       <c r="E57" s="3">
-        <v>43446</v>
+        <v>42466</v>
       </c>
       <c r="F57" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4014,13 +3962,13 @@
         <v>7659</v>
       </c>
       <c r="E58" s="3">
-        <v>43446</v>
+        <v>42466</v>
       </c>
       <c r="F58" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4034,13 +3982,13 @@
         <v>277</v>
       </c>
       <c r="E59" s="3">
-        <v>43452</v>
+        <v>42472</v>
       </c>
       <c r="F59" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4054,13 +4002,13 @@
         <v>235</v>
       </c>
       <c r="E60" s="3">
-        <v>43457</v>
+        <v>42477</v>
       </c>
       <c r="F60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4074,13 +4022,13 @@
         <v>1113</v>
       </c>
       <c r="E61" s="3">
-        <v>43458</v>
+        <v>42478</v>
       </c>
       <c r="F61" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4094,13 +4042,13 @@
         <v>1128</v>
       </c>
       <c r="E62" s="3">
-        <v>43461</v>
+        <v>42481</v>
       </c>
       <c r="F62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4114,13 +4062,13 @@
         <v>9231</v>
       </c>
       <c r="E63" s="3">
-        <v>43462</v>
+        <v>42482</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4134,13 +4082,13 @@
         <v>4387</v>
       </c>
       <c r="E64" s="3">
-        <v>43463</v>
+        <v>42483</v>
       </c>
       <c r="F64" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4154,13 +4102,13 @@
         <v>2763</v>
       </c>
       <c r="E65" s="3">
-        <v>43465</v>
+        <v>42485</v>
       </c>
       <c r="F65" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4174,13 +4122,13 @@
         <v>7898</v>
       </c>
       <c r="E66" s="3">
-        <v>43467</v>
+        <v>42487</v>
       </c>
       <c r="F66" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4194,13 +4142,13 @@
         <v>2427</v>
       </c>
       <c r="E67" s="3">
-        <v>43470</v>
+        <v>42490</v>
       </c>
       <c r="F67" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4214,13 +4162,13 @@
         <v>8663</v>
       </c>
       <c r="E68" s="3">
-        <v>43471</v>
+        <v>42491</v>
       </c>
       <c r="F68" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4234,13 +4182,13 @@
         <v>2789</v>
       </c>
       <c r="E69" s="3">
-        <v>43471</v>
+        <v>42491</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4254,13 +4202,13 @@
         <v>4054</v>
       </c>
       <c r="E70" s="3">
-        <v>43472</v>
+        <v>42492</v>
       </c>
       <c r="F70" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4274,13 +4222,13 @@
         <v>2262</v>
       </c>
       <c r="E71" s="3">
-        <v>43472</v>
+        <v>42492</v>
       </c>
       <c r="F71" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4294,13 +4242,13 @@
         <v>5600</v>
       </c>
       <c r="E72" s="3">
-        <v>43472</v>
+        <v>42492</v>
       </c>
       <c r="F72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4314,13 +4262,13 @@
         <v>5787</v>
       </c>
       <c r="E73" s="3">
-        <v>43473</v>
+        <v>42493</v>
       </c>
       <c r="F73" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4334,13 +4282,13 @@
         <v>6295</v>
       </c>
       <c r="E74" s="3">
-        <v>43473</v>
+        <v>42493</v>
       </c>
       <c r="F74" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4354,13 +4302,13 @@
         <v>474</v>
       </c>
       <c r="E75" s="3">
-        <v>43475</v>
+        <v>42495</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4374,13 +4322,13 @@
         <v>4325</v>
       </c>
       <c r="E76" s="3">
-        <v>43475</v>
+        <v>42495</v>
       </c>
       <c r="F76" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4394,13 +4342,13 @@
         <v>592</v>
       </c>
       <c r="E77" s="3">
-        <v>43476</v>
+        <v>42496</v>
       </c>
       <c r="F77" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4414,13 +4362,13 @@
         <v>4330</v>
       </c>
       <c r="E78" s="3">
-        <v>43478</v>
+        <v>42498</v>
       </c>
       <c r="F78" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4434,13 +4382,13 @@
         <v>9405</v>
       </c>
       <c r="E79" s="3">
-        <v>43478</v>
+        <v>42498</v>
       </c>
       <c r="F79" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4454,13 +4402,13 @@
         <v>7671</v>
       </c>
       <c r="E80" s="3">
-        <v>43478</v>
+        <v>42498</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4474,13 +4422,13 @@
         <v>5791</v>
       </c>
       <c r="E81" s="3">
-        <v>43478</v>
+        <v>42498</v>
       </c>
       <c r="F81" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4494,13 +4442,13 @@
         <v>6007</v>
       </c>
       <c r="E82" s="3">
-        <v>43482</v>
+        <v>42502</v>
       </c>
       <c r="F82" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4514,13 +4462,13 @@
         <v>5030</v>
       </c>
       <c r="E83" s="3">
-        <v>43484</v>
+        <v>42504</v>
       </c>
       <c r="F83" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4534,13 +4482,13 @@
         <v>6763</v>
       </c>
       <c r="E84" s="3">
-        <v>43484</v>
+        <v>42504</v>
       </c>
       <c r="F84" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4554,13 +4502,13 @@
         <v>4248</v>
       </c>
       <c r="E85" s="3">
-        <v>43485</v>
+        <v>42505</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4574,13 +4522,13 @@
         <v>9543</v>
       </c>
       <c r="E86" s="3">
-        <v>43486</v>
+        <v>42506</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4594,13 +4542,13 @@
         <v>2054</v>
       </c>
       <c r="E87" s="3">
-        <v>43486</v>
+        <v>42506</v>
       </c>
       <c r="F87" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4614,13 +4562,13 @@
         <v>7094</v>
       </c>
       <c r="E88" s="3">
-        <v>43486</v>
+        <v>42506</v>
       </c>
       <c r="F88" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4634,13 +4582,13 @@
         <v>6087</v>
       </c>
       <c r="E89" s="3">
-        <v>43488</v>
+        <v>42508</v>
       </c>
       <c r="F89" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4654,13 +4602,13 @@
         <v>4264</v>
       </c>
       <c r="E90" s="3">
-        <v>43489</v>
+        <v>42509</v>
       </c>
       <c r="F90" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4674,13 +4622,13 @@
         <v>9333</v>
       </c>
       <c r="E91" s="3">
-        <v>43490</v>
+        <v>42510</v>
       </c>
       <c r="F91" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4694,13 +4642,13 @@
         <v>8775</v>
       </c>
       <c r="E92" s="3">
-        <v>43492</v>
+        <v>42512</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4714,13 +4662,13 @@
         <v>2011</v>
       </c>
       <c r="E93" s="3">
-        <v>43493</v>
+        <v>42513</v>
       </c>
       <c r="F93" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4734,13 +4682,13 @@
         <v>5632</v>
       </c>
       <c r="E94" s="3">
-        <v>43495</v>
+        <v>42515</v>
       </c>
       <c r="F94" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4754,13 +4702,13 @@
         <v>4904</v>
       </c>
       <c r="E95" s="3">
-        <v>43495</v>
+        <v>42515</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4774,13 +4722,13 @@
         <v>1002</v>
       </c>
       <c r="E96" s="3">
-        <v>43495</v>
+        <v>42515</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4794,13 +4742,13 @@
         <v>8141</v>
       </c>
       <c r="E97" s="3">
-        <v>43496</v>
+        <v>42516</v>
       </c>
       <c r="F97" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4814,13 +4762,13 @@
         <v>3644</v>
       </c>
       <c r="E98" s="3">
-        <v>43496</v>
+        <v>42516</v>
       </c>
       <c r="F98" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4834,13 +4782,13 @@
         <v>1380</v>
       </c>
       <c r="E99" s="3">
-        <v>43496</v>
+        <v>42516</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4854,13 +4802,13 @@
         <v>8354</v>
       </c>
       <c r="E100" s="3">
-        <v>43496</v>
+        <v>42516</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4874,13 +4822,13 @@
         <v>5182</v>
       </c>
       <c r="E101" s="3">
-        <v>43497</v>
+        <v>42517</v>
       </c>
       <c r="F101" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4894,13 +4842,13 @@
         <v>2193</v>
       </c>
       <c r="E102" s="3">
-        <v>43497</v>
+        <v>42517</v>
       </c>
       <c r="F102" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4914,13 +4862,13 @@
         <v>3647</v>
       </c>
       <c r="E103" s="3">
-        <v>43498</v>
+        <v>42518</v>
       </c>
       <c r="F103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4934,13 +4882,13 @@
         <v>4104</v>
       </c>
       <c r="E104" s="3">
-        <v>43498</v>
+        <v>42518</v>
       </c>
       <c r="F104" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4954,13 +4902,13 @@
         <v>7457</v>
       </c>
       <c r="E105" s="3">
-        <v>43498</v>
+        <v>42518</v>
       </c>
       <c r="F105" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4974,13 +4922,13 @@
         <v>3767</v>
       </c>
       <c r="E106" s="3">
-        <v>43499</v>
+        <v>42519</v>
       </c>
       <c r="F106" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4994,13 +4942,13 @@
         <v>4685</v>
       </c>
       <c r="E107" s="3">
-        <v>43500</v>
+        <v>42520</v>
       </c>
       <c r="F107" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>107</v>
       </c>
@@ -5014,13 +4962,13 @@
         <v>3917</v>
       </c>
       <c r="E108" s="3">
-        <v>43505</v>
+        <v>42525</v>
       </c>
       <c r="F108" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>108</v>
       </c>
@@ -5034,13 +4982,13 @@
         <v>521</v>
       </c>
       <c r="E109" s="3">
-        <v>43505</v>
+        <v>42525</v>
       </c>
       <c r="F109" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5054,13 +5002,13 @@
         <v>5605</v>
       </c>
       <c r="E110" s="3">
-        <v>43511</v>
+        <v>42531</v>
       </c>
       <c r="F110" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5074,13 +5022,13 @@
         <v>9630</v>
       </c>
       <c r="E111" s="3">
-        <v>43512</v>
+        <v>42532</v>
       </c>
       <c r="F111" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5094,13 +5042,13 @@
         <v>6941</v>
       </c>
       <c r="E112" s="3">
-        <v>43521</v>
+        <v>42541</v>
       </c>
       <c r="F112" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5114,13 +5062,13 @@
         <v>7231</v>
       </c>
       <c r="E113" s="3">
-        <v>43521</v>
+        <v>42541</v>
       </c>
       <c r="F113" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5134,13 +5082,13 @@
         <v>8891</v>
       </c>
       <c r="E114" s="3">
-        <v>43524</v>
+        <v>42544</v>
       </c>
       <c r="F114" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5154,13 +5102,13 @@
         <v>107</v>
       </c>
       <c r="E115" s="3">
-        <v>43526</v>
+        <v>42546</v>
       </c>
       <c r="F115" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5174,13 +5122,13 @@
         <v>4243</v>
       </c>
       <c r="E116" s="3">
-        <v>43527</v>
+        <v>42547</v>
       </c>
       <c r="F116" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5194,13 +5142,13 @@
         <v>4514</v>
       </c>
       <c r="E117" s="3">
-        <v>43528</v>
+        <v>42548</v>
       </c>
       <c r="F117" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5214,13 +5162,13 @@
         <v>5480</v>
       </c>
       <c r="E118" s="3">
-        <v>43533</v>
+        <v>42553</v>
       </c>
       <c r="F118" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5234,13 +5182,13 @@
         <v>5002</v>
       </c>
       <c r="E119" s="3">
-        <v>43533</v>
+        <v>42553</v>
       </c>
       <c r="F119" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5254,13 +5202,13 @@
         <v>8530</v>
       </c>
       <c r="E120" s="3">
-        <v>43536</v>
+        <v>42556</v>
       </c>
       <c r="F120" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5274,13 +5222,13 @@
         <v>4819</v>
       </c>
       <c r="E121" s="3">
-        <v>43538</v>
+        <v>42558</v>
       </c>
       <c r="F121" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5294,13 +5242,13 @@
         <v>6343</v>
       </c>
       <c r="E122" s="3">
-        <v>43542</v>
+        <v>42562</v>
       </c>
       <c r="F122" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5314,13 +5262,13 @@
         <v>2318</v>
       </c>
       <c r="E123" s="3">
-        <v>43544</v>
+        <v>42564</v>
       </c>
       <c r="F123" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5334,13 +5282,13 @@
         <v>220</v>
       </c>
       <c r="E124" s="3">
-        <v>43551</v>
+        <v>42571</v>
       </c>
       <c r="F124" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5354,13 +5302,13 @@
         <v>6341</v>
       </c>
       <c r="E125" s="3">
-        <v>43551</v>
+        <v>42571</v>
       </c>
       <c r="F125" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5374,13 +5322,13 @@
         <v>330</v>
       </c>
       <c r="E126" s="3">
-        <v>43551</v>
+        <v>42571</v>
       </c>
       <c r="F126" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5394,13 +5342,13 @@
         <v>3027</v>
       </c>
       <c r="E127" s="3">
-        <v>43551</v>
+        <v>42571</v>
       </c>
       <c r="F127" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5414,13 +5362,13 @@
         <v>850</v>
       </c>
       <c r="E128" s="3">
-        <v>43553</v>
+        <v>42573</v>
       </c>
       <c r="F128" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5434,13 +5382,13 @@
         <v>8986</v>
       </c>
       <c r="E129" s="3">
-        <v>43554</v>
+        <v>42574</v>
       </c>
       <c r="F129" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5454,13 +5402,13 @@
         <v>3800</v>
       </c>
       <c r="E130" s="3">
-        <v>43556</v>
+        <v>42576</v>
       </c>
       <c r="F130" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5474,13 +5422,13 @@
         <v>5751</v>
       </c>
       <c r="E131" s="3">
-        <v>43559</v>
+        <v>42579</v>
       </c>
       <c r="F131" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5494,13 +5442,13 @@
         <v>1704</v>
       </c>
       <c r="E132" s="3">
-        <v>43560</v>
+        <v>42580</v>
       </c>
       <c r="F132" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5514,13 +5462,13 @@
         <v>7966</v>
       </c>
       <c r="E133" s="3">
-        <v>43561</v>
+        <v>42581</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5534,13 +5482,13 @@
         <v>852</v>
       </c>
       <c r="E134" s="3">
-        <v>43562</v>
+        <v>42582</v>
       </c>
       <c r="F134" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5554,13 +5502,13 @@
         <v>8416</v>
       </c>
       <c r="E135" s="3">
-        <v>43562</v>
+        <v>42582</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5574,13 +5522,13 @@
         <v>7144</v>
       </c>
       <c r="E136" s="3">
-        <v>43563</v>
+        <v>42583</v>
       </c>
       <c r="F136" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5594,13 +5542,13 @@
         <v>7854</v>
       </c>
       <c r="E137" s="3">
-        <v>43563</v>
+        <v>42583</v>
       </c>
       <c r="F137" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5614,13 +5562,13 @@
         <v>859</v>
       </c>
       <c r="E138" s="3">
-        <v>43565</v>
+        <v>42585</v>
       </c>
       <c r="F138" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5634,13 +5582,13 @@
         <v>8049</v>
       </c>
       <c r="E139" s="3">
-        <v>43574</v>
+        <v>42594</v>
       </c>
       <c r="F139" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5654,13 +5602,13 @@
         <v>2836</v>
       </c>
       <c r="E140" s="3">
-        <v>43575</v>
+        <v>42595</v>
       </c>
       <c r="F140" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5674,13 +5622,13 @@
         <v>1743</v>
       </c>
       <c r="E141" s="3">
-        <v>43581</v>
+        <v>42601</v>
       </c>
       <c r="F141" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5694,13 +5642,13 @@
         <v>3844</v>
       </c>
       <c r="E142" s="3">
-        <v>43585</v>
+        <v>42605</v>
       </c>
       <c r="F142" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5714,13 +5662,13 @@
         <v>7490</v>
       </c>
       <c r="E143" s="3">
-        <v>43586</v>
+        <v>42606</v>
       </c>
       <c r="F143" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5734,13 +5682,13 @@
         <v>4483</v>
       </c>
       <c r="E144" s="3">
-        <v>43587</v>
+        <v>42607</v>
       </c>
       <c r="F144" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5754,13 +5702,13 @@
         <v>7333</v>
       </c>
       <c r="E145" s="3">
-        <v>43589</v>
+        <v>42609</v>
       </c>
       <c r="F145" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5774,13 +5722,13 @@
         <v>7654</v>
       </c>
       <c r="E146" s="3">
-        <v>43590</v>
+        <v>42610</v>
       </c>
       <c r="F146" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5794,13 +5742,13 @@
         <v>3944</v>
       </c>
       <c r="E147" s="3">
-        <v>43591</v>
+        <v>42611</v>
       </c>
       <c r="F147" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5814,13 +5762,13 @@
         <v>5761</v>
       </c>
       <c r="E148" s="3">
-        <v>43591</v>
+        <v>42611</v>
       </c>
       <c r="F148" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5834,13 +5782,13 @@
         <v>6864</v>
       </c>
       <c r="E149" s="3">
-        <v>43594</v>
+        <v>42614</v>
       </c>
       <c r="F149" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5854,13 +5802,13 @@
         <v>4016</v>
       </c>
       <c r="E150" s="3">
-        <v>43594</v>
+        <v>42614</v>
       </c>
       <c r="F150" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5874,13 +5822,13 @@
         <v>1841</v>
       </c>
       <c r="E151" s="3">
-        <v>43595</v>
+        <v>42615</v>
       </c>
       <c r="F151" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5894,13 +5842,13 @@
         <v>424</v>
       </c>
       <c r="E152" s="3">
-        <v>43598</v>
+        <v>42618</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5914,13 +5862,13 @@
         <v>8765</v>
       </c>
       <c r="E153" s="3">
-        <v>43600</v>
+        <v>42620</v>
       </c>
       <c r="F153" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5934,13 +5882,13 @@
         <v>5583</v>
       </c>
       <c r="E154" s="3">
-        <v>43601</v>
+        <v>42621</v>
       </c>
       <c r="F154" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5954,13 +5902,13 @@
         <v>4390</v>
       </c>
       <c r="E155" s="3">
-        <v>43602</v>
+        <v>42622</v>
       </c>
       <c r="F155" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5974,13 +5922,13 @@
         <v>352</v>
       </c>
       <c r="E156" s="3">
-        <v>43602</v>
+        <v>42622</v>
       </c>
       <c r="F156" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5994,13 +5942,13 @@
         <v>8489</v>
       </c>
       <c r="E157" s="3">
-        <v>43604</v>
+        <v>42624</v>
       </c>
       <c r="F157" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6014,13 +5962,13 @@
         <v>7090</v>
       </c>
       <c r="E158" s="3">
-        <v>43604</v>
+        <v>42624</v>
       </c>
       <c r="F158" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6034,13 +5982,13 @@
         <v>7880</v>
       </c>
       <c r="E159" s="3">
-        <v>43608</v>
+        <v>42628</v>
       </c>
       <c r="F159" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6054,13 +6002,13 @@
         <v>3861</v>
       </c>
       <c r="E160" s="3">
-        <v>43611</v>
+        <v>42631</v>
       </c>
       <c r="F160" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6074,13 +6022,13 @@
         <v>7927</v>
       </c>
       <c r="E161" s="3">
-        <v>43612</v>
+        <v>42632</v>
       </c>
       <c r="F161" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6094,13 +6042,13 @@
         <v>6162</v>
       </c>
       <c r="E162" s="3">
-        <v>43613</v>
+        <v>42633</v>
       </c>
       <c r="F162" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6114,13 +6062,13 @@
         <v>5523</v>
       </c>
       <c r="E163" s="3">
-        <v>43618</v>
+        <v>42638</v>
       </c>
       <c r="F163" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6134,13 +6082,13 @@
         <v>5936</v>
       </c>
       <c r="E164" s="3">
-        <v>43618</v>
+        <v>42638</v>
       </c>
       <c r="F164" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6154,13 +6102,13 @@
         <v>7251</v>
       </c>
       <c r="E165" s="3">
-        <v>43619</v>
+        <v>42639</v>
       </c>
       <c r="F165" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6174,13 +6122,13 @@
         <v>6187</v>
       </c>
       <c r="E166" s="3">
-        <v>43620</v>
+        <v>42640</v>
       </c>
       <c r="F166" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6194,13 +6142,13 @@
         <v>3210</v>
       </c>
       <c r="E167" s="3">
-        <v>43622</v>
+        <v>42642</v>
       </c>
       <c r="F167" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6214,13 +6162,13 @@
         <v>682</v>
       </c>
       <c r="E168" s="3">
-        <v>43622</v>
+        <v>42642</v>
       </c>
       <c r="F168" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6234,13 +6182,13 @@
         <v>793</v>
       </c>
       <c r="E169" s="3">
-        <v>43626</v>
+        <v>42646</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6254,13 +6202,13 @@
         <v>5346</v>
       </c>
       <c r="E170" s="3">
-        <v>43627</v>
+        <v>42647</v>
       </c>
       <c r="F170" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6274,13 +6222,13 @@
         <v>7103</v>
       </c>
       <c r="E171" s="3">
-        <v>43630</v>
+        <v>42650</v>
       </c>
       <c r="F171" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6294,13 +6242,13 @@
         <v>4603</v>
       </c>
       <c r="E172" s="3">
-        <v>43633</v>
+        <v>42653</v>
       </c>
       <c r="F172" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6314,13 +6262,13 @@
         <v>8160</v>
       </c>
       <c r="E173" s="3">
-        <v>43639</v>
+        <v>42659</v>
       </c>
       <c r="F173" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6334,13 +6282,13 @@
         <v>7171</v>
       </c>
       <c r="E174" s="3">
-        <v>43646</v>
+        <v>42666</v>
       </c>
       <c r="F174" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6354,13 +6302,13 @@
         <v>3552</v>
       </c>
       <c r="E175" s="3">
-        <v>43646</v>
+        <v>42666</v>
       </c>
       <c r="F175" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6374,13 +6322,13 @@
         <v>7273</v>
       </c>
       <c r="E176" s="3">
-        <v>43648</v>
+        <v>42668</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6394,13 +6342,13 @@
         <v>2402</v>
       </c>
       <c r="E177" s="3">
-        <v>43649</v>
+        <v>42669</v>
       </c>
       <c r="F177" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6414,13 +6362,13 @@
         <v>1197</v>
       </c>
       <c r="E178" s="3">
-        <v>43649</v>
+        <v>42669</v>
       </c>
       <c r="F178" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6434,13 +6382,13 @@
         <v>5015</v>
       </c>
       <c r="E179" s="3">
-        <v>43649</v>
+        <v>42669</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6454,13 +6402,13 @@
         <v>5818</v>
       </c>
       <c r="E180" s="3">
-        <v>43656</v>
+        <v>42676</v>
       </c>
       <c r="F180" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6474,13 +6422,13 @@
         <v>4399</v>
       </c>
       <c r="E181" s="3">
-        <v>43657</v>
+        <v>42677</v>
       </c>
       <c r="F181" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6494,13 +6442,13 @@
         <v>3011</v>
       </c>
       <c r="E182" s="3">
-        <v>43657</v>
+        <v>42677</v>
       </c>
       <c r="F182" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>182</v>
       </c>
@@ -6514,13 +6462,13 @@
         <v>4715</v>
       </c>
       <c r="E183" s="3">
-        <v>43663</v>
+        <v>42683</v>
       </c>
       <c r="F183" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6534,13 +6482,13 @@
         <v>5321</v>
       </c>
       <c r="E184" s="3">
-        <v>43666</v>
+        <v>42686</v>
       </c>
       <c r="F184" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6554,13 +6502,13 @@
         <v>8894</v>
       </c>
       <c r="E185" s="3">
-        <v>43669</v>
+        <v>42689</v>
       </c>
       <c r="F185" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6574,13 +6522,13 @@
         <v>4846</v>
       </c>
       <c r="E186" s="3">
-        <v>43679</v>
+        <v>42699</v>
       </c>
       <c r="F186" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6594,13 +6542,13 @@
         <v>284</v>
       </c>
       <c r="E187" s="3">
-        <v>43679</v>
+        <v>42699</v>
       </c>
       <c r="F187" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>187</v>
       </c>
@@ -6614,13 +6562,13 @@
         <v>8283</v>
       </c>
       <c r="E188" s="3">
-        <v>43680</v>
+        <v>42700</v>
       </c>
       <c r="F188" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6634,13 +6582,13 @@
         <v>9990</v>
       </c>
       <c r="E189" s="3">
-        <v>43682</v>
+        <v>42702</v>
       </c>
       <c r="F189" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6654,13 +6602,13 @@
         <v>9014</v>
       </c>
       <c r="E190" s="3">
-        <v>43682</v>
+        <v>42702</v>
       </c>
       <c r="F190" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>190</v>
       </c>
@@ -6674,13 +6622,13 @@
         <v>1942</v>
       </c>
       <c r="E191" s="3">
-        <v>43683</v>
+        <v>42703</v>
       </c>
       <c r="F191" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6694,13 +6642,13 @@
         <v>7223</v>
       </c>
       <c r="E192" s="3">
-        <v>43684</v>
+        <v>42704</v>
       </c>
       <c r="F192" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6714,13 +6662,13 @@
         <v>4673</v>
       </c>
       <c r="E193" s="3">
-        <v>43686</v>
+        <v>42706</v>
       </c>
       <c r="F193" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6734,13 +6682,13 @@
         <v>9104</v>
       </c>
       <c r="E194" s="3">
-        <v>43688</v>
+        <v>42708</v>
       </c>
       <c r="F194" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6754,13 +6702,13 @@
         <v>6078</v>
       </c>
       <c r="E195" s="3">
-        <v>43689</v>
+        <v>42709</v>
       </c>
       <c r="F195" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6774,13 +6722,13 @@
         <v>3278</v>
       </c>
       <c r="E196" s="3">
-        <v>43690</v>
+        <v>42710</v>
       </c>
       <c r="F196" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6794,13 +6742,13 @@
         <v>136</v>
       </c>
       <c r="E197" s="3">
-        <v>43696</v>
+        <v>42716</v>
       </c>
       <c r="F197" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6814,13 +6762,13 @@
         <v>8377</v>
       </c>
       <c r="E198" s="3">
-        <v>43696</v>
+        <v>42716</v>
       </c>
       <c r="F198" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6834,13 +6782,13 @@
         <v>2382</v>
       </c>
       <c r="E199" s="3">
-        <v>43696</v>
+        <v>42716</v>
       </c>
       <c r="F199" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6854,13 +6802,13 @@
         <v>8702</v>
       </c>
       <c r="E200" s="3">
-        <v>43699</v>
+        <v>42719</v>
       </c>
       <c r="F200" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6874,13 +6822,13 @@
         <v>5021</v>
       </c>
       <c r="E201" s="3">
-        <v>43700</v>
+        <v>42720</v>
       </c>
       <c r="F201" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6894,13 +6842,13 @@
         <v>1760</v>
       </c>
       <c r="E202" s="3">
-        <v>43700</v>
+        <v>42720</v>
       </c>
       <c r="F202" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6914,13 +6862,13 @@
         <v>4766</v>
       </c>
       <c r="E203" s="3">
-        <v>43702</v>
+        <v>42722</v>
       </c>
       <c r="F203" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6934,13 +6882,13 @@
         <v>1541</v>
       </c>
       <c r="E204" s="3">
-        <v>43703</v>
+        <v>42723</v>
       </c>
       <c r="F204" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6954,13 +6902,13 @@
         <v>2782</v>
       </c>
       <c r="E205" s="3">
-        <v>43704</v>
+        <v>42724</v>
       </c>
       <c r="F205" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6974,13 +6922,13 @@
         <v>2455</v>
       </c>
       <c r="E206" s="3">
-        <v>43704</v>
+        <v>42724</v>
       </c>
       <c r="F206" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6994,13 +6942,13 @@
         <v>4512</v>
       </c>
       <c r="E207" s="3">
-        <v>43706</v>
+        <v>42726</v>
       </c>
       <c r="F207" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>207</v>
       </c>
@@ -7014,13 +6962,13 @@
         <v>8752</v>
       </c>
       <c r="E208" s="3">
-        <v>43706</v>
+        <v>42726</v>
       </c>
       <c r="F208" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>208</v>
       </c>
@@ -7034,13 +6982,13 @@
         <v>9127</v>
       </c>
       <c r="E209" s="3">
-        <v>43709</v>
+        <v>42729</v>
       </c>
       <c r="F209" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>209</v>
       </c>
@@ -7054,13 +7002,13 @@
         <v>1777</v>
       </c>
       <c r="E210" s="3">
-        <v>43712</v>
+        <v>42732</v>
       </c>
       <c r="F210" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>210</v>
       </c>
@@ -7074,13 +7022,13 @@
         <v>680</v>
       </c>
       <c r="E211" s="3">
-        <v>43712</v>
+        <v>42732</v>
       </c>
       <c r="F211" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>211</v>
       </c>
@@ -7094,13 +7042,13 @@
         <v>958</v>
       </c>
       <c r="E212" s="3">
-        <v>43713</v>
+        <v>42733</v>
       </c>
       <c r="F212" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>212</v>
       </c>
@@ -7114,13 +7062,13 @@
         <v>2613</v>
       </c>
       <c r="E213" s="3">
-        <v>43713</v>
+        <v>42733</v>
       </c>
       <c r="F213" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>213</v>
       </c>
@@ -7134,7 +7082,7 @@
         <v>339</v>
       </c>
       <c r="E214" s="3">
-        <v>43714</v>
+        <v>42734</v>
       </c>
       <c r="F214" t="s">
         <v>10</v>
@@ -7143,26 +7091,25 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" customWidth="1"/>
+    <col min="2" max="2" width="12.46484375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -7170,7 +7117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -7181,7 +7128,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -7192,7 +7139,7 @@
         <v>8892</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -7203,7 +7150,7 @@
         <v>9543</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -7214,7 +7161,7 @@
         <v>8416</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -7225,7 +7172,7 @@
         <v>9630</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -7236,7 +7183,7 @@
         <v>9127</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -7247,7 +7194,7 @@
         <v>9333</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -7258,7 +7205,7 @@
         <v>9990</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -7267,16 +7214,6 @@
       </c>
       <c r="C12" s="4">
         <v>9990</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -7285,18 +7222,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7304,7 +7243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -7312,13 +7251,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -7326,7 +7265,7 @@
         <v>191257</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -7334,7 +7273,7 @@
         <v>340295</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -7342,7 +7281,7 @@
         <v>57079</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -7350,7 +7289,7 @@
         <v>104438</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
@@ -7358,13 +7297,13 @@
         <v>693069</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
@@ -7372,7 +7311,7 @@
         <v>57281</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -7380,7 +7319,7 @@
         <v>142439</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -7388,7 +7327,7 @@
         <v>136945</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -7396,7 +7335,7 @@
         <v>336665</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Updating Unit 1.3 activities
</commit_message>
<xml_diff>
--- a/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/02-Ins_PivotTables/Solved/PivotTables.xlsx
+++ b/01-Class-Activities/Mon-Wed-Class/01-Excel/3/Activities/02-Ins_PivotTables/Solved/PivotTables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacob\OneDrive\Documents\WorkAndSchool\TeachingAssistant\DataViz\DataViz-Lesson-Plans\01-Lesson-Plans\01-Excel\2\Activities\09-Ins_PivotTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98452\Documents\GitHub\GWU-ARL-DATA-PT-09-2019-U-C\01-Class-Activities\Mon-Wed-Class\01-Excel\3\Activities\02-Ins_PivotTables\Solved\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="EB38C96A757F5A8F8FDBBC133FE1386DB659D6FE" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{B87C83CC-A6C0-4333-8D1D-521D4EE6FF64}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="20183" windowHeight="12818" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20190" windowHeight="12825" tabRatio="796"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,13 +19,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$214</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="31">
   <si>
     <t>Country</t>
   </si>
@@ -124,15 +123,21 @@
   <si>
     <t>Vegetables Total</t>
   </si>
+  <si>
+    <t>Can someone remind me how to do number formatting again?</t>
+  </si>
+  <si>
+    <t>I nominate Keishacarr! (You have to say her first and last name together) :-)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +147,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -182,11 +195,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -211,9 +250,9 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{FE0D9BC4-DAB8-496C-B826-44D3B596CAFA}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="4"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -228,7 +267,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jacob's Gaming Rig" refreshedDate="42873.827209490744" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="213" xr:uid="{00000000-000A-0000-FFFF-FFFF09000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Jacob's Gaming Rig" refreshedDate="42873.827209490744" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="213">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F214" sheet="Sheet1"/>
   </cacheSource>
@@ -2140,7 +2179,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -2392,7 +2431,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -2491,6 +2530,21 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F214" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F214"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Order ID"/>
+    <tableColumn id="2" name="Product"/>
+    <tableColumn id="3" name="Category"/>
+    <tableColumn id="4" name="Profit" dataDxfId="2"/>
+    <tableColumn id="5" name="Date" dataDxfId="1"/>
+    <tableColumn id="6" name="Country"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2789,26 +2843,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.46484375" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2828,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2842,13 +2894,13 @@
         <v>4270</v>
       </c>
       <c r="E2" s="3">
-        <v>42375</v>
+        <v>43355</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2862,13 +2914,13 @@
         <v>8239</v>
       </c>
       <c r="E3" s="3">
-        <v>42376</v>
+        <v>43356</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2882,13 +2934,13 @@
         <v>617</v>
       </c>
       <c r="E4" s="3">
-        <v>42377</v>
+        <v>43357</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2902,13 +2954,13 @@
         <v>8384</v>
       </c>
       <c r="E5" s="3">
-        <v>42379</v>
+        <v>43359</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2922,13 +2974,13 @@
         <v>2626</v>
       </c>
       <c r="E6" s="3">
-        <v>42379</v>
+        <v>43359</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2942,13 +2994,13 @@
         <v>3610</v>
       </c>
       <c r="E7" s="3">
-        <v>42380</v>
+        <v>43360</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2962,13 +3014,13 @@
         <v>9062</v>
       </c>
       <c r="E8" s="3">
-        <v>42380</v>
+        <v>43360</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2982,13 +3034,13 @@
         <v>6906</v>
       </c>
       <c r="E9" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3002,13 +3054,13 @@
         <v>2417</v>
       </c>
       <c r="E10" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3022,13 +3074,13 @@
         <v>7431</v>
       </c>
       <c r="E11" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3042,13 +3094,13 @@
         <v>8250</v>
       </c>
       <c r="E12" s="3">
-        <v>42385</v>
+        <v>43365</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3062,13 +3114,13 @@
         <v>7012</v>
       </c>
       <c r="E13" s="3">
-        <v>42387</v>
+        <v>43367</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3082,13 +3134,13 @@
         <v>1903</v>
       </c>
       <c r="E14" s="3">
-        <v>42389</v>
+        <v>43369</v>
       </c>
       <c r="F14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3102,13 +3154,13 @@
         <v>2824</v>
       </c>
       <c r="E15" s="3">
-        <v>42391</v>
+        <v>43371</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3122,13 +3174,13 @@
         <v>6946</v>
       </c>
       <c r="E16" s="3">
-        <v>42393</v>
+        <v>43373</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3142,13 +3194,13 @@
         <v>2320</v>
       </c>
       <c r="E17" s="3">
-        <v>42396</v>
+        <v>43376</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3162,13 +3214,13 @@
         <v>2116</v>
       </c>
       <c r="E18" s="3">
-        <v>42397</v>
+        <v>43377</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3182,13 +3234,13 @@
         <v>1135</v>
       </c>
       <c r="E19" s="3">
-        <v>42399</v>
+        <v>43379</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3202,13 +3254,13 @@
         <v>3595</v>
       </c>
       <c r="E20" s="3">
-        <v>42399</v>
+        <v>43379</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3222,13 +3274,13 @@
         <v>1161</v>
       </c>
       <c r="E21" s="3">
-        <v>42402</v>
+        <v>43382</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3242,13 +3294,13 @@
         <v>2256</v>
       </c>
       <c r="E22" s="3">
-        <v>42404</v>
+        <v>43384</v>
       </c>
       <c r="F22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3262,13 +3314,13 @@
         <v>1004</v>
       </c>
       <c r="E23" s="3">
-        <v>42411</v>
+        <v>43391</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3282,13 +3334,13 @@
         <v>3642</v>
       </c>
       <c r="E24" s="3">
-        <v>42414</v>
+        <v>43394</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3302,13 +3354,13 @@
         <v>4582</v>
       </c>
       <c r="E25" s="3">
-        <v>42417</v>
+        <v>43397</v>
       </c>
       <c r="F25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3322,13 +3374,13 @@
         <v>3559</v>
       </c>
       <c r="E26" s="3">
-        <v>42417</v>
+        <v>43397</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3342,13 +3394,13 @@
         <v>5154</v>
       </c>
       <c r="E27" s="3">
-        <v>42417</v>
+        <v>43397</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3362,13 +3414,13 @@
         <v>7388</v>
       </c>
       <c r="E28" s="3">
-        <v>42418</v>
+        <v>43398</v>
       </c>
       <c r="F28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3382,13 +3434,13 @@
         <v>7163</v>
       </c>
       <c r="E29" s="3">
-        <v>42418</v>
+        <v>43398</v>
       </c>
       <c r="F29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3402,13 +3454,13 @@
         <v>5101</v>
       </c>
       <c r="E30" s="3">
-        <v>42420</v>
+        <v>43400</v>
       </c>
       <c r="F30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3422,13 +3474,13 @@
         <v>7602</v>
       </c>
       <c r="E31" s="3">
-        <v>42421</v>
+        <v>43401</v>
       </c>
       <c r="F31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3442,13 +3494,13 @@
         <v>1641</v>
       </c>
       <c r="E32" s="3">
-        <v>42422</v>
+        <v>43402</v>
       </c>
       <c r="F32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3462,13 +3514,13 @@
         <v>8892</v>
       </c>
       <c r="E33" s="3">
-        <v>42423</v>
+        <v>43403</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3482,13 +3534,13 @@
         <v>2060</v>
       </c>
       <c r="E34" s="3">
-        <v>42429</v>
+        <v>43409</v>
       </c>
       <c r="F34" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3502,13 +3554,13 @@
         <v>1557</v>
       </c>
       <c r="E35" s="3">
-        <v>42429</v>
+        <v>43409</v>
       </c>
       <c r="F35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3522,13 +3574,13 @@
         <v>6509</v>
       </c>
       <c r="E36" s="3">
-        <v>42430</v>
+        <v>43410</v>
       </c>
       <c r="F36" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3542,13 +3594,13 @@
         <v>5718</v>
       </c>
       <c r="E37" s="3">
-        <v>42433</v>
+        <v>43413</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3562,13 +3614,13 @@
         <v>7655</v>
       </c>
       <c r="E38" s="3">
-        <v>42434</v>
+        <v>43414</v>
       </c>
       <c r="F38" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3582,13 +3634,13 @@
         <v>9116</v>
       </c>
       <c r="E39" s="3">
-        <v>42434</v>
+        <v>43414</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3602,13 +3654,13 @@
         <v>2795</v>
       </c>
       <c r="E40" s="3">
-        <v>42444</v>
+        <v>43424</v>
       </c>
       <c r="F40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3622,13 +3674,13 @@
         <v>5084</v>
       </c>
       <c r="E41" s="3">
-        <v>42444</v>
+        <v>43424</v>
       </c>
       <c r="F41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3642,13 +3694,13 @@
         <v>8941</v>
       </c>
       <c r="E42" s="3">
-        <v>42444</v>
+        <v>43424</v>
       </c>
       <c r="F42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3662,13 +3714,13 @@
         <v>5341</v>
       </c>
       <c r="E43" s="3">
-        <v>42445</v>
+        <v>43425</v>
       </c>
       <c r="F43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3682,13 +3734,13 @@
         <v>135</v>
       </c>
       <c r="E44" s="3">
-        <v>42448</v>
+        <v>43428</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3702,13 +3754,13 @@
         <v>9400</v>
       </c>
       <c r="E45" s="3">
-        <v>42448</v>
+        <v>43428</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3722,13 +3774,13 @@
         <v>6045</v>
       </c>
       <c r="E46" s="3">
-        <v>42450</v>
+        <v>43430</v>
       </c>
       <c r="F46" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3742,13 +3794,13 @@
         <v>5820</v>
       </c>
       <c r="E47" s="3">
-        <v>42451</v>
+        <v>43431</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3762,13 +3814,13 @@
         <v>8887</v>
       </c>
       <c r="E48" s="3">
-        <v>42452</v>
+        <v>43432</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3782,13 +3834,13 @@
         <v>6982</v>
       </c>
       <c r="E49" s="3">
-        <v>42453</v>
+        <v>43433</v>
       </c>
       <c r="F49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3802,13 +3854,13 @@
         <v>4029</v>
       </c>
       <c r="E50" s="3">
-        <v>42455</v>
+        <v>43435</v>
       </c>
       <c r="F50" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3822,13 +3874,13 @@
         <v>3665</v>
       </c>
       <c r="E51" s="3">
-        <v>42455</v>
+        <v>43435</v>
       </c>
       <c r="F51" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3842,13 +3894,13 @@
         <v>4781</v>
       </c>
       <c r="E52" s="3">
-        <v>42458</v>
+        <v>43438</v>
       </c>
       <c r="F52" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3862,13 +3914,13 @@
         <v>3663</v>
       </c>
       <c r="E53" s="3">
-        <v>42459</v>
+        <v>43439</v>
       </c>
       <c r="F53" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3882,13 +3934,13 @@
         <v>6331</v>
       </c>
       <c r="E54" s="3">
-        <v>42461</v>
+        <v>43441</v>
       </c>
       <c r="F54" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3902,13 +3954,13 @@
         <v>4364</v>
       </c>
       <c r="E55" s="3">
-        <v>42461</v>
+        <v>43441</v>
       </c>
       <c r="F55" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3922,13 +3974,13 @@
         <v>607</v>
       </c>
       <c r="E56" s="3">
-        <v>42463</v>
+        <v>43443</v>
       </c>
       <c r="F56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3942,13 +3994,13 @@
         <v>1054</v>
       </c>
       <c r="E57" s="3">
-        <v>42466</v>
+        <v>43446</v>
       </c>
       <c r="F57" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3962,13 +4014,13 @@
         <v>7659</v>
       </c>
       <c r="E58" s="3">
-        <v>42466</v>
+        <v>43446</v>
       </c>
       <c r="F58" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3982,13 +4034,13 @@
         <v>277</v>
       </c>
       <c r="E59" s="3">
-        <v>42472</v>
+        <v>43452</v>
       </c>
       <c r="F59" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4002,13 +4054,13 @@
         <v>235</v>
       </c>
       <c r="E60" s="3">
-        <v>42477</v>
+        <v>43457</v>
       </c>
       <c r="F60" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4022,13 +4074,13 @@
         <v>1113</v>
       </c>
       <c r="E61" s="3">
-        <v>42478</v>
+        <v>43458</v>
       </c>
       <c r="F61" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4042,13 +4094,13 @@
         <v>1128</v>
       </c>
       <c r="E62" s="3">
-        <v>42481</v>
+        <v>43461</v>
       </c>
       <c r="F62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4062,13 +4114,13 @@
         <v>9231</v>
       </c>
       <c r="E63" s="3">
-        <v>42482</v>
+        <v>43462</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4082,13 +4134,13 @@
         <v>4387</v>
       </c>
       <c r="E64" s="3">
-        <v>42483</v>
+        <v>43463</v>
       </c>
       <c r="F64" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4102,13 +4154,13 @@
         <v>2763</v>
       </c>
       <c r="E65" s="3">
-        <v>42485</v>
+        <v>43465</v>
       </c>
       <c r="F65" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4122,13 +4174,13 @@
         <v>7898</v>
       </c>
       <c r="E66" s="3">
-        <v>42487</v>
+        <v>43467</v>
       </c>
       <c r="F66" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4142,13 +4194,13 @@
         <v>2427</v>
       </c>
       <c r="E67" s="3">
-        <v>42490</v>
+        <v>43470</v>
       </c>
       <c r="F67" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4162,13 +4214,13 @@
         <v>8663</v>
       </c>
       <c r="E68" s="3">
-        <v>42491</v>
+        <v>43471</v>
       </c>
       <c r="F68" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4182,13 +4234,13 @@
         <v>2789</v>
       </c>
       <c r="E69" s="3">
-        <v>42491</v>
+        <v>43471</v>
       </c>
       <c r="F69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4202,13 +4254,13 @@
         <v>4054</v>
       </c>
       <c r="E70" s="3">
-        <v>42492</v>
+        <v>43472</v>
       </c>
       <c r="F70" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4222,13 +4274,13 @@
         <v>2262</v>
       </c>
       <c r="E71" s="3">
-        <v>42492</v>
+        <v>43472</v>
       </c>
       <c r="F71" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4242,13 +4294,13 @@
         <v>5600</v>
       </c>
       <c r="E72" s="3">
-        <v>42492</v>
+        <v>43472</v>
       </c>
       <c r="F72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4262,13 +4314,13 @@
         <v>5787</v>
       </c>
       <c r="E73" s="3">
-        <v>42493</v>
+        <v>43473</v>
       </c>
       <c r="F73" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4282,13 +4334,13 @@
         <v>6295</v>
       </c>
       <c r="E74" s="3">
-        <v>42493</v>
+        <v>43473</v>
       </c>
       <c r="F74" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4302,13 +4354,13 @@
         <v>474</v>
       </c>
       <c r="E75" s="3">
-        <v>42495</v>
+        <v>43475</v>
       </c>
       <c r="F75" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4322,13 +4374,13 @@
         <v>4325</v>
       </c>
       <c r="E76" s="3">
-        <v>42495</v>
+        <v>43475</v>
       </c>
       <c r="F76" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4342,13 +4394,13 @@
         <v>592</v>
       </c>
       <c r="E77" s="3">
-        <v>42496</v>
+        <v>43476</v>
       </c>
       <c r="F77" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4362,13 +4414,13 @@
         <v>4330</v>
       </c>
       <c r="E78" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F78" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4382,13 +4434,13 @@
         <v>9405</v>
       </c>
       <c r="E79" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F79" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4402,13 +4454,13 @@
         <v>7671</v>
       </c>
       <c r="E80" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F80" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4422,13 +4474,13 @@
         <v>5791</v>
       </c>
       <c r="E81" s="3">
-        <v>42498</v>
+        <v>43478</v>
       </c>
       <c r="F81" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -4442,13 +4494,13 @@
         <v>6007</v>
       </c>
       <c r="E82" s="3">
-        <v>42502</v>
+        <v>43482</v>
       </c>
       <c r="F82" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -4462,13 +4514,13 @@
         <v>5030</v>
       </c>
       <c r="E83" s="3">
-        <v>42504</v>
+        <v>43484</v>
       </c>
       <c r="F83" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -4482,13 +4534,13 @@
         <v>6763</v>
       </c>
       <c r="E84" s="3">
-        <v>42504</v>
+        <v>43484</v>
       </c>
       <c r="F84" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -4502,13 +4554,13 @@
         <v>4248</v>
       </c>
       <c r="E85" s="3">
-        <v>42505</v>
+        <v>43485</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -4522,13 +4574,13 @@
         <v>9543</v>
       </c>
       <c r="E86" s="3">
-        <v>42506</v>
+        <v>43486</v>
       </c>
       <c r="F86" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -4542,13 +4594,13 @@
         <v>2054</v>
       </c>
       <c r="E87" s="3">
-        <v>42506</v>
+        <v>43486</v>
       </c>
       <c r="F87" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -4562,13 +4614,13 @@
         <v>7094</v>
       </c>
       <c r="E88" s="3">
-        <v>42506</v>
+        <v>43486</v>
       </c>
       <c r="F88" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -4582,13 +4634,13 @@
         <v>6087</v>
       </c>
       <c r="E89" s="3">
-        <v>42508</v>
+        <v>43488</v>
       </c>
       <c r="F89" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4602,13 +4654,13 @@
         <v>4264</v>
       </c>
       <c r="E90" s="3">
-        <v>42509</v>
+        <v>43489</v>
       </c>
       <c r="F90" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4622,13 +4674,13 @@
         <v>9333</v>
       </c>
       <c r="E91" s="3">
-        <v>42510</v>
+        <v>43490</v>
       </c>
       <c r="F91" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4642,13 +4694,13 @@
         <v>8775</v>
       </c>
       <c r="E92" s="3">
-        <v>42512</v>
+        <v>43492</v>
       </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4662,13 +4714,13 @@
         <v>2011</v>
       </c>
       <c r="E93" s="3">
-        <v>42513</v>
+        <v>43493</v>
       </c>
       <c r="F93" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4682,13 +4734,13 @@
         <v>5632</v>
       </c>
       <c r="E94" s="3">
-        <v>42515</v>
+        <v>43495</v>
       </c>
       <c r="F94" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4702,13 +4754,13 @@
         <v>4904</v>
       </c>
       <c r="E95" s="3">
-        <v>42515</v>
+        <v>43495</v>
       </c>
       <c r="F95" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4722,13 +4774,13 @@
         <v>1002</v>
       </c>
       <c r="E96" s="3">
-        <v>42515</v>
+        <v>43495</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4742,13 +4794,13 @@
         <v>8141</v>
       </c>
       <c r="E97" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F97" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4762,13 +4814,13 @@
         <v>3644</v>
       </c>
       <c r="E98" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F98" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4782,13 +4834,13 @@
         <v>1380</v>
       </c>
       <c r="E99" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4802,13 +4854,13 @@
         <v>8354</v>
       </c>
       <c r="E100" s="3">
-        <v>42516</v>
+        <v>43496</v>
       </c>
       <c r="F100" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4822,13 +4874,13 @@
         <v>5182</v>
       </c>
       <c r="E101" s="3">
-        <v>42517</v>
+        <v>43497</v>
       </c>
       <c r="F101" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4842,13 +4894,13 @@
         <v>2193</v>
       </c>
       <c r="E102" s="3">
-        <v>42517</v>
+        <v>43497</v>
       </c>
       <c r="F102" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4862,13 +4914,13 @@
         <v>3647</v>
       </c>
       <c r="E103" s="3">
-        <v>42518</v>
+        <v>43498</v>
       </c>
       <c r="F103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4882,13 +4934,13 @@
         <v>4104</v>
       </c>
       <c r="E104" s="3">
-        <v>42518</v>
+        <v>43498</v>
       </c>
       <c r="F104" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4902,13 +4954,13 @@
         <v>7457</v>
       </c>
       <c r="E105" s="3">
-        <v>42518</v>
+        <v>43498</v>
       </c>
       <c r="F105" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4922,13 +4974,13 @@
         <v>3767</v>
       </c>
       <c r="E106" s="3">
-        <v>42519</v>
+        <v>43499</v>
       </c>
       <c r="F106" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4942,13 +4994,13 @@
         <v>4685</v>
       </c>
       <c r="E107" s="3">
-        <v>42520</v>
+        <v>43500</v>
       </c>
       <c r="F107" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4962,13 +5014,13 @@
         <v>3917</v>
       </c>
       <c r="E108" s="3">
-        <v>42525</v>
+        <v>43505</v>
       </c>
       <c r="F108" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4982,13 +5034,13 @@
         <v>521</v>
       </c>
       <c r="E109" s="3">
-        <v>42525</v>
+        <v>43505</v>
       </c>
       <c r="F109" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -5002,13 +5054,13 @@
         <v>5605</v>
       </c>
       <c r="E110" s="3">
-        <v>42531</v>
+        <v>43511</v>
       </c>
       <c r="F110" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -5022,13 +5074,13 @@
         <v>9630</v>
       </c>
       <c r="E111" s="3">
-        <v>42532</v>
+        <v>43512</v>
       </c>
       <c r="F111" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -5042,13 +5094,13 @@
         <v>6941</v>
       </c>
       <c r="E112" s="3">
-        <v>42541</v>
+        <v>43521</v>
       </c>
       <c r="F112" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -5062,13 +5114,13 @@
         <v>7231</v>
       </c>
       <c r="E113" s="3">
-        <v>42541</v>
+        <v>43521</v>
       </c>
       <c r="F113" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -5082,13 +5134,13 @@
         <v>8891</v>
       </c>
       <c r="E114" s="3">
-        <v>42544</v>
+        <v>43524</v>
       </c>
       <c r="F114" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -5102,13 +5154,13 @@
         <v>107</v>
       </c>
       <c r="E115" s="3">
-        <v>42546</v>
+        <v>43526</v>
       </c>
       <c r="F115" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -5122,13 +5174,13 @@
         <v>4243</v>
       </c>
       <c r="E116" s="3">
-        <v>42547</v>
+        <v>43527</v>
       </c>
       <c r="F116" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -5142,13 +5194,13 @@
         <v>4514</v>
       </c>
       <c r="E117" s="3">
-        <v>42548</v>
+        <v>43528</v>
       </c>
       <c r="F117" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -5162,13 +5214,13 @@
         <v>5480</v>
       </c>
       <c r="E118" s="3">
-        <v>42553</v>
+        <v>43533</v>
       </c>
       <c r="F118" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5182,13 +5234,13 @@
         <v>5002</v>
       </c>
       <c r="E119" s="3">
-        <v>42553</v>
+        <v>43533</v>
       </c>
       <c r="F119" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5202,13 +5254,13 @@
         <v>8530</v>
       </c>
       <c r="E120" s="3">
-        <v>42556</v>
+        <v>43536</v>
       </c>
       <c r="F120" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5222,13 +5274,13 @@
         <v>4819</v>
       </c>
       <c r="E121" s="3">
-        <v>42558</v>
+        <v>43538</v>
       </c>
       <c r="F121" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5242,13 +5294,13 @@
         <v>6343</v>
       </c>
       <c r="E122" s="3">
-        <v>42562</v>
+        <v>43542</v>
       </c>
       <c r="F122" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5262,13 +5314,13 @@
         <v>2318</v>
       </c>
       <c r="E123" s="3">
-        <v>42564</v>
+        <v>43544</v>
       </c>
       <c r="F123" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5282,13 +5334,13 @@
         <v>220</v>
       </c>
       <c r="E124" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F124" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5302,13 +5354,13 @@
         <v>6341</v>
       </c>
       <c r="E125" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F125" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5322,13 +5374,13 @@
         <v>330</v>
       </c>
       <c r="E126" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F126" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5342,13 +5394,13 @@
         <v>3027</v>
       </c>
       <c r="E127" s="3">
-        <v>42571</v>
+        <v>43551</v>
       </c>
       <c r="F127" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5362,13 +5414,13 @@
         <v>850</v>
       </c>
       <c r="E128" s="3">
-        <v>42573</v>
+        <v>43553</v>
       </c>
       <c r="F128" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5382,13 +5434,13 @@
         <v>8986</v>
       </c>
       <c r="E129" s="3">
-        <v>42574</v>
+        <v>43554</v>
       </c>
       <c r="F129" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5402,13 +5454,13 @@
         <v>3800</v>
       </c>
       <c r="E130" s="3">
-        <v>42576</v>
+        <v>43556</v>
       </c>
       <c r="F130" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5422,13 +5474,13 @@
         <v>5751</v>
       </c>
       <c r="E131" s="3">
-        <v>42579</v>
+        <v>43559</v>
       </c>
       <c r="F131" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5442,13 +5494,13 @@
         <v>1704</v>
       </c>
       <c r="E132" s="3">
-        <v>42580</v>
+        <v>43560</v>
       </c>
       <c r="F132" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5462,13 +5514,13 @@
         <v>7966</v>
       </c>
       <c r="E133" s="3">
-        <v>42581</v>
+        <v>43561</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5482,13 +5534,13 @@
         <v>852</v>
       </c>
       <c r="E134" s="3">
-        <v>42582</v>
+        <v>43562</v>
       </c>
       <c r="F134" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5502,13 +5554,13 @@
         <v>8416</v>
       </c>
       <c r="E135" s="3">
-        <v>42582</v>
+        <v>43562</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5522,13 +5574,13 @@
         <v>7144</v>
       </c>
       <c r="E136" s="3">
-        <v>42583</v>
+        <v>43563</v>
       </c>
       <c r="F136" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5542,13 +5594,13 @@
         <v>7854</v>
       </c>
       <c r="E137" s="3">
-        <v>42583</v>
+        <v>43563</v>
       </c>
       <c r="F137" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5562,13 +5614,13 @@
         <v>859</v>
       </c>
       <c r="E138" s="3">
-        <v>42585</v>
+        <v>43565</v>
       </c>
       <c r="F138" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5582,13 +5634,13 @@
         <v>8049</v>
       </c>
       <c r="E139" s="3">
-        <v>42594</v>
+        <v>43574</v>
       </c>
       <c r="F139" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5602,13 +5654,13 @@
         <v>2836</v>
       </c>
       <c r="E140" s="3">
-        <v>42595</v>
+        <v>43575</v>
       </c>
       <c r="F140" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5622,13 +5674,13 @@
         <v>1743</v>
       </c>
       <c r="E141" s="3">
-        <v>42601</v>
+        <v>43581</v>
       </c>
       <c r="F141" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5642,13 +5694,13 @@
         <v>3844</v>
       </c>
       <c r="E142" s="3">
-        <v>42605</v>
+        <v>43585</v>
       </c>
       <c r="F142" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5662,13 +5714,13 @@
         <v>7490</v>
       </c>
       <c r="E143" s="3">
-        <v>42606</v>
+        <v>43586</v>
       </c>
       <c r="F143" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5682,13 +5734,13 @@
         <v>4483</v>
       </c>
       <c r="E144" s="3">
-        <v>42607</v>
+        <v>43587</v>
       </c>
       <c r="F144" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5702,13 +5754,13 @@
         <v>7333</v>
       </c>
       <c r="E145" s="3">
-        <v>42609</v>
+        <v>43589</v>
       </c>
       <c r="F145" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5722,13 +5774,13 @@
         <v>7654</v>
       </c>
       <c r="E146" s="3">
-        <v>42610</v>
+        <v>43590</v>
       </c>
       <c r="F146" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5742,13 +5794,13 @@
         <v>3944</v>
       </c>
       <c r="E147" s="3">
-        <v>42611</v>
+        <v>43591</v>
       </c>
       <c r="F147" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5762,13 +5814,13 @@
         <v>5761</v>
       </c>
       <c r="E148" s="3">
-        <v>42611</v>
+        <v>43591</v>
       </c>
       <c r="F148" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5782,13 +5834,13 @@
         <v>6864</v>
       </c>
       <c r="E149" s="3">
-        <v>42614</v>
+        <v>43594</v>
       </c>
       <c r="F149" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5802,13 +5854,13 @@
         <v>4016</v>
       </c>
       <c r="E150" s="3">
-        <v>42614</v>
+        <v>43594</v>
       </c>
       <c r="F150" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5822,13 +5874,13 @@
         <v>1841</v>
       </c>
       <c r="E151" s="3">
-        <v>42615</v>
+        <v>43595</v>
       </c>
       <c r="F151" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5842,13 +5894,13 @@
         <v>424</v>
       </c>
       <c r="E152" s="3">
-        <v>42618</v>
+        <v>43598</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5862,13 +5914,13 @@
         <v>8765</v>
       </c>
       <c r="E153" s="3">
-        <v>42620</v>
+        <v>43600</v>
       </c>
       <c r="F153" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5882,13 +5934,13 @@
         <v>5583</v>
       </c>
       <c r="E154" s="3">
-        <v>42621</v>
+        <v>43601</v>
       </c>
       <c r="F154" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5902,13 +5954,13 @@
         <v>4390</v>
       </c>
       <c r="E155" s="3">
-        <v>42622</v>
+        <v>43602</v>
       </c>
       <c r="F155" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5922,13 +5974,13 @@
         <v>352</v>
       </c>
       <c r="E156" s="3">
-        <v>42622</v>
+        <v>43602</v>
       </c>
       <c r="F156" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5942,13 +5994,13 @@
         <v>8489</v>
       </c>
       <c r="E157" s="3">
-        <v>42624</v>
+        <v>43604</v>
       </c>
       <c r="F157" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5962,13 +6014,13 @@
         <v>7090</v>
       </c>
       <c r="E158" s="3">
-        <v>42624</v>
+        <v>43604</v>
       </c>
       <c r="F158" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5982,13 +6034,13 @@
         <v>7880</v>
       </c>
       <c r="E159" s="3">
-        <v>42628</v>
+        <v>43608</v>
       </c>
       <c r="F159" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6002,13 +6054,13 @@
         <v>3861</v>
       </c>
       <c r="E160" s="3">
-        <v>42631</v>
+        <v>43611</v>
       </c>
       <c r="F160" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6022,13 +6074,13 @@
         <v>7927</v>
       </c>
       <c r="E161" s="3">
-        <v>42632</v>
+        <v>43612</v>
       </c>
       <c r="F161" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6042,13 +6094,13 @@
         <v>6162</v>
       </c>
       <c r="E162" s="3">
-        <v>42633</v>
+        <v>43613</v>
       </c>
       <c r="F162" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6062,13 +6114,13 @@
         <v>5523</v>
       </c>
       <c r="E163" s="3">
-        <v>42638</v>
+        <v>43618</v>
       </c>
       <c r="F163" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6082,13 +6134,13 @@
         <v>5936</v>
       </c>
       <c r="E164" s="3">
-        <v>42638</v>
+        <v>43618</v>
       </c>
       <c r="F164" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6102,13 +6154,13 @@
         <v>7251</v>
       </c>
       <c r="E165" s="3">
-        <v>42639</v>
+        <v>43619</v>
       </c>
       <c r="F165" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6122,13 +6174,13 @@
         <v>6187</v>
       </c>
       <c r="E166" s="3">
-        <v>42640</v>
+        <v>43620</v>
       </c>
       <c r="F166" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6142,13 +6194,13 @@
         <v>3210</v>
       </c>
       <c r="E167" s="3">
-        <v>42642</v>
+        <v>43622</v>
       </c>
       <c r="F167" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6162,13 +6214,13 @@
         <v>682</v>
       </c>
       <c r="E168" s="3">
-        <v>42642</v>
+        <v>43622</v>
       </c>
       <c r="F168" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6182,13 +6234,13 @@
         <v>793</v>
       </c>
       <c r="E169" s="3">
-        <v>42646</v>
+        <v>43626</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6202,13 +6254,13 @@
         <v>5346</v>
       </c>
       <c r="E170" s="3">
-        <v>42647</v>
+        <v>43627</v>
       </c>
       <c r="F170" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6222,13 +6274,13 @@
         <v>7103</v>
       </c>
       <c r="E171" s="3">
-        <v>42650</v>
+        <v>43630</v>
       </c>
       <c r="F171" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6242,13 +6294,13 @@
         <v>4603</v>
       </c>
       <c r="E172" s="3">
-        <v>42653</v>
+        <v>43633</v>
       </c>
       <c r="F172" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6262,13 +6314,13 @@
         <v>8160</v>
       </c>
       <c r="E173" s="3">
-        <v>42659</v>
+        <v>43639</v>
       </c>
       <c r="F173" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6282,13 +6334,13 @@
         <v>7171</v>
       </c>
       <c r="E174" s="3">
-        <v>42666</v>
+        <v>43646</v>
       </c>
       <c r="F174" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6302,13 +6354,13 @@
         <v>3552</v>
       </c>
       <c r="E175" s="3">
-        <v>42666</v>
+        <v>43646</v>
       </c>
       <c r="F175" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -6322,13 +6374,13 @@
         <v>7273</v>
       </c>
       <c r="E176" s="3">
-        <v>42668</v>
+        <v>43648</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -6342,13 +6394,13 @@
         <v>2402</v>
       </c>
       <c r="E177" s="3">
-        <v>42669</v>
+        <v>43649</v>
       </c>
       <c r="F177" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -6362,13 +6414,13 @@
         <v>1197</v>
       </c>
       <c r="E178" s="3">
-        <v>42669</v>
+        <v>43649</v>
       </c>
       <c r="F178" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -6382,13 +6434,13 @@
         <v>5015</v>
       </c>
       <c r="E179" s="3">
-        <v>42669</v>
+        <v>43649</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -6402,13 +6454,13 @@
         <v>5818</v>
       </c>
       <c r="E180" s="3">
-        <v>42676</v>
+        <v>43656</v>
       </c>
       <c r="F180" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -6422,13 +6474,13 @@
         <v>4399</v>
       </c>
       <c r="E181" s="3">
-        <v>42677</v>
+        <v>43657</v>
       </c>
       <c r="F181" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -6442,13 +6494,13 @@
         <v>3011</v>
       </c>
       <c r="E182" s="3">
-        <v>42677</v>
+        <v>43657</v>
       </c>
       <c r="F182" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -6462,13 +6514,13 @@
         <v>4715</v>
       </c>
       <c r="E183" s="3">
-        <v>42683</v>
+        <v>43663</v>
       </c>
       <c r="F183" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -6482,13 +6534,13 @@
         <v>5321</v>
       </c>
       <c r="E184" s="3">
-        <v>42686</v>
+        <v>43666</v>
       </c>
       <c r="F184" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -6502,13 +6554,13 @@
         <v>8894</v>
       </c>
       <c r="E185" s="3">
-        <v>42689</v>
+        <v>43669</v>
       </c>
       <c r="F185" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -6522,13 +6574,13 @@
         <v>4846</v>
       </c>
       <c r="E186" s="3">
-        <v>42699</v>
+        <v>43679</v>
       </c>
       <c r="F186" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -6542,13 +6594,13 @@
         <v>284</v>
       </c>
       <c r="E187" s="3">
-        <v>42699</v>
+        <v>43679</v>
       </c>
       <c r="F187" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -6562,13 +6614,13 @@
         <v>8283</v>
       </c>
       <c r="E188" s="3">
-        <v>42700</v>
+        <v>43680</v>
       </c>
       <c r="F188" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -6582,13 +6634,13 @@
         <v>9990</v>
       </c>
       <c r="E189" s="3">
-        <v>42702</v>
+        <v>43682</v>
       </c>
       <c r="F189" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -6602,13 +6654,13 @@
         <v>9014</v>
       </c>
       <c r="E190" s="3">
-        <v>42702</v>
+        <v>43682</v>
       </c>
       <c r="F190" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -6622,13 +6674,13 @@
         <v>1942</v>
       </c>
       <c r="E191" s="3">
-        <v>42703</v>
+        <v>43683</v>
       </c>
       <c r="F191" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -6642,13 +6694,13 @@
         <v>7223</v>
       </c>
       <c r="E192" s="3">
-        <v>42704</v>
+        <v>43684</v>
       </c>
       <c r="F192" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -6662,13 +6714,13 @@
         <v>4673</v>
       </c>
       <c r="E193" s="3">
-        <v>42706</v>
+        <v>43686</v>
       </c>
       <c r="F193" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -6682,13 +6734,13 @@
         <v>9104</v>
       </c>
       <c r="E194" s="3">
-        <v>42708</v>
+        <v>43688</v>
       </c>
       <c r="F194" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6702,13 +6754,13 @@
         <v>6078</v>
       </c>
       <c r="E195" s="3">
-        <v>42709</v>
+        <v>43689</v>
       </c>
       <c r="F195" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6722,13 +6774,13 @@
         <v>3278</v>
       </c>
       <c r="E196" s="3">
-        <v>42710</v>
+        <v>43690</v>
       </c>
       <c r="F196" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6742,13 +6794,13 @@
         <v>136</v>
       </c>
       <c r="E197" s="3">
-        <v>42716</v>
+        <v>43696</v>
       </c>
       <c r="F197" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6762,13 +6814,13 @@
         <v>8377</v>
       </c>
       <c r="E198" s="3">
-        <v>42716</v>
+        <v>43696</v>
       </c>
       <c r="F198" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6782,13 +6834,13 @@
         <v>2382</v>
       </c>
       <c r="E199" s="3">
-        <v>42716</v>
+        <v>43696</v>
       </c>
       <c r="F199" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6802,13 +6854,13 @@
         <v>8702</v>
       </c>
       <c r="E200" s="3">
-        <v>42719</v>
+        <v>43699</v>
       </c>
       <c r="F200" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6822,13 +6874,13 @@
         <v>5021</v>
       </c>
       <c r="E201" s="3">
-        <v>42720</v>
+        <v>43700</v>
       </c>
       <c r="F201" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6842,13 +6894,13 @@
         <v>1760</v>
       </c>
       <c r="E202" s="3">
-        <v>42720</v>
+        <v>43700</v>
       </c>
       <c r="F202" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6862,13 +6914,13 @@
         <v>4766</v>
       </c>
       <c r="E203" s="3">
-        <v>42722</v>
+        <v>43702</v>
       </c>
       <c r="F203" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6882,13 +6934,13 @@
         <v>1541</v>
       </c>
       <c r="E204" s="3">
-        <v>42723</v>
+        <v>43703</v>
       </c>
       <c r="F204" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6902,13 +6954,13 @@
         <v>2782</v>
       </c>
       <c r="E205" s="3">
-        <v>42724</v>
+        <v>43704</v>
       </c>
       <c r="F205" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6922,13 +6974,13 @@
         <v>2455</v>
       </c>
       <c r="E206" s="3">
-        <v>42724</v>
+        <v>43704</v>
       </c>
       <c r="F206" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6942,13 +6994,13 @@
         <v>4512</v>
       </c>
       <c r="E207" s="3">
-        <v>42726</v>
+        <v>43706</v>
       </c>
       <c r="F207" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6962,13 +7014,13 @@
         <v>8752</v>
       </c>
       <c r="E208" s="3">
-        <v>42726</v>
+        <v>43706</v>
       </c>
       <c r="F208" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6982,13 +7034,13 @@
         <v>9127</v>
       </c>
       <c r="E209" s="3">
-        <v>42729</v>
+        <v>43709</v>
       </c>
       <c r="F209" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -7002,13 +7054,13 @@
         <v>1777</v>
       </c>
       <c r="E210" s="3">
-        <v>42732</v>
+        <v>43712</v>
       </c>
       <c r="F210" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -7022,13 +7074,13 @@
         <v>680</v>
       </c>
       <c r="E211" s="3">
-        <v>42732</v>
+        <v>43712</v>
       </c>
       <c r="F211" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -7042,13 +7094,13 @@
         <v>958</v>
       </c>
       <c r="E212" s="3">
-        <v>42733</v>
+        <v>43713</v>
       </c>
       <c r="F212" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -7062,13 +7114,13 @@
         <v>2613</v>
       </c>
       <c r="E213" s="3">
-        <v>42733</v>
+        <v>43713</v>
       </c>
       <c r="F213" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -7082,7 +7134,7 @@
         <v>339</v>
       </c>
       <c r="E214" s="3">
-        <v>42734</v>
+        <v>43714</v>
       </c>
       <c r="F214" t="s">
         <v>10</v>
@@ -7091,25 +7143,26 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -7117,7 +7170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
@@ -7128,7 +7181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -7139,7 +7192,7 @@
         <v>8892</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -7150,7 +7203,7 @@
         <v>9543</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -7161,7 +7214,7 @@
         <v>8416</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -7172,7 +7225,7 @@
         <v>9630</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -7183,7 +7236,7 @@
         <v>9127</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -7194,7 +7247,7 @@
         <v>9333</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -7205,7 +7258,7 @@
         <v>9990</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -7214,6 +7267,16 @@
       </c>
       <c r="C12" s="4">
         <v>9990</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -7222,20 +7285,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="12.46484375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7243,7 +7304,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -7251,13 +7312,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -7265,7 +7326,7 @@
         <v>191257</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -7273,7 +7334,7 @@
         <v>340295</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -7281,7 +7342,7 @@
         <v>57079</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -7289,7 +7350,7 @@
         <v>104438</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>27</v>
       </c>
@@ -7297,13 +7358,13 @@
         <v>693069</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
@@ -7311,7 +7372,7 @@
         <v>57281</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
@@ -7319,7 +7380,7 @@
         <v>142439</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -7327,7 +7388,7 @@
         <v>136945</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -7335,7 +7396,7 @@
         <v>336665</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>